<commit_message>
Update Gantt, added Airtfoil Integrated test
</commit_message>
<xml_diff>
--- a/gantt_chart_update.xlsx
+++ b/gantt_chart_update.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mlawson/Documents/GitHub/hfm_integration_demonstration_plan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcmania\Documents\GitHub\hfm_integration_demonstration_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C8EDC6-C416-584C-A497-779626EB1FE8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="460" windowWidth="32460" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="465" windowWidth="32460" windowHeight="20535" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ECP Integration &amp; Demonstration" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="4" r:id="rId2"/>
     <sheet name="ValidationCases" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="187">
   <si>
     <t>1.1.1</t>
   </si>
@@ -464,19 +463,7 @@
     <t>Uncertinity and coordination between the ABL team and the integration/demo team is needed</t>
   </si>
   <si>
-    <t>Months</t>
-  </si>
-  <si>
-    <t>FTE</t>
-  </si>
-  <si>
     <t>Wake Dynamics</t>
-  </si>
-  <si>
-    <t>Total Task 1+2 months</t>
-  </si>
-  <si>
-    <t>Total Task 1+2 FTE</t>
   </si>
   <si>
     <t>3.1.13</t>
@@ -573,17 +560,75 @@
       <t>[Critical, work will be performed in ABL area]</t>
     </r>
   </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>Person Months</t>
+  </si>
+  <si>
+    <t>4.1.0</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>Integrated Airfoil Analysis</t>
+  </si>
+  <si>
+    <t>Compile wind tunnel test data from literature</t>
+  </si>
+  <si>
+    <t>Mesh each airfoil and analyze in 2D or quasi-2D in Nalu</t>
+  </si>
+  <si>
+    <t>4.1.3</t>
+  </si>
+  <si>
+    <t>Quantify error and propagate to blade/rotor</t>
+  </si>
+  <si>
+    <t>Hybrid RANS-LES tests 1 airfoil, no unsteady</t>
+  </si>
+  <si>
+    <t>Maniaci</t>
+  </si>
+  <si>
+    <t>Blaylock / Maniaci/ Lawson</t>
+  </si>
+  <si>
+    <t>Compare to wind tunnel data, report results</t>
+  </si>
+  <si>
+    <t>4.1.4</t>
+  </si>
+  <si>
+    <t>Total PM</t>
+  </si>
+  <si>
+    <t>Total FTE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="11">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -649,20 +694,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -696,13 +733,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -894,51 +926,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -949,29 +1037,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -980,90 +1068,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="5" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Calculation" xfId="5" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1340,155 +1433,155 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL324"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AL330"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC51" sqref="AC51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="8.5" customWidth="1"/>
-    <col min="2" max="2" width="67.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.83203125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="36.1640625" style="68" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.125" customWidth="1"/>
+    <col min="3" max="3" width="23.375" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="36.125" style="68" customWidth="1"/>
+    <col min="7" max="7" width="4.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.875" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.5" style="5" customWidth="1"/>
-    <col min="10" max="10" width="3.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.625" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.875" style="5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.5" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.125" style="5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="4" style="5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="4.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.875" style="5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="4" style="5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="4.5" style="5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="4" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="3.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="4.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.83203125" customWidth="1"/>
+    <col min="32" max="32" width="4.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="2" customFormat="1" ht="19">
+    <row r="1" spans="1:38" s="2" customFormat="1" ht="18.75">
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="63"/>
-      <c r="G1" s="88" t="s">
+      <c r="G1" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87" t="s">
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87" t="s">
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="93"/>
+      <c r="R1" s="93"/>
+      <c r="S1" s="93"/>
+      <c r="T1" s="93"/>
+      <c r="U1" s="93"/>
+      <c r="V1" s="93"/>
+      <c r="W1" s="93"/>
+      <c r="X1" s="93"/>
+      <c r="Y1" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
-      <c r="AD1" s="87"/>
-      <c r="AE1" s="87"/>
-      <c r="AF1" s="87"/>
-      <c r="AG1" s="87"/>
-      <c r="AH1" s="87"/>
-      <c r="AI1" s="87"/>
-      <c r="AJ1" s="87"/>
-    </row>
-    <row r="2" spans="1:38" s="2" customFormat="1" ht="19">
+      <c r="Z1" s="93"/>
+      <c r="AA1" s="93"/>
+      <c r="AB1" s="93"/>
+      <c r="AC1" s="93"/>
+      <c r="AD1" s="93"/>
+      <c r="AE1" s="93"/>
+      <c r="AF1" s="93"/>
+      <c r="AG1" s="93"/>
+      <c r="AH1" s="93"/>
+      <c r="AI1" s="93"/>
+      <c r="AJ1" s="93"/>
+    </row>
+    <row r="2" spans="1:38" s="2" customFormat="1" ht="18.75">
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="63"/>
-      <c r="G2" s="89" t="s">
+      <c r="G2" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="91" t="s">
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="89"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="89" t="s">
+      <c r="K2" s="95"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="89"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="91" t="s">
+      <c r="N2" s="95"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="90"/>
-      <c r="S2" s="91" t="s">
+      <c r="Q2" s="95"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="89"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="91" t="s">
+      <c r="T2" s="95"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="89"/>
-      <c r="X2" s="90"/>
-      <c r="Y2" s="89" t="s">
+      <c r="W2" s="95"/>
+      <c r="X2" s="96"/>
+      <c r="Y2" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="89"/>
-      <c r="AA2" s="90"/>
-      <c r="AB2" s="89" t="s">
+      <c r="Z2" s="95"/>
+      <c r="AA2" s="96"/>
+      <c r="AB2" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="AC2" s="89"/>
-      <c r="AD2" s="90"/>
-      <c r="AE2" s="91" t="s">
+      <c r="AC2" s="95"/>
+      <c r="AD2" s="96"/>
+      <c r="AE2" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="AF2" s="89"/>
-      <c r="AG2" s="90"/>
-      <c r="AH2" s="89" t="s">
+      <c r="AF2" s="95"/>
+      <c r="AG2" s="96"/>
+      <c r="AH2" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="AI2" s="89"/>
-      <c r="AJ2" s="90"/>
-    </row>
-    <row r="3" spans="1:38" s="2" customFormat="1" ht="19">
+      <c r="AI2" s="95"/>
+      <c r="AJ2" s="96"/>
+    </row>
+    <row r="3" spans="1:38" s="2" customFormat="1" ht="18.75">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1595,7 +1688,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="48">
+    <row r="4" spans="1:38" ht="47.25">
       <c r="A4" s="23" t="s">
         <v>15</v>
       </c>
@@ -1652,8 +1745,12 @@
         <v>51</v>
       </c>
       <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="62"/>
+      <c r="E5" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="62" t="s">
+        <v>170</v>
+      </c>
       <c r="G5" s="52"/>
       <c r="H5" s="53"/>
       <c r="I5"/>
@@ -1697,8 +1794,12 @@
         <v>83</v>
       </c>
       <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="47"/>
+      <c r="E6" s="32">
+        <v>1</v>
+      </c>
+      <c r="F6" s="62" t="s">
+        <v>170</v>
+      </c>
       <c r="G6" s="12"/>
       <c r="H6" s="53"/>
       <c r="I6" s="54"/>
@@ -1799,7 +1900,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="85" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="8"/>
@@ -1832,7 +1933,7 @@
       <c r="AI8" s="8"/>
       <c r="AJ8" s="14"/>
     </row>
-    <row r="9" spans="1:38" s="59" customFormat="1" ht="32">
+    <row r="9" spans="1:38" s="59" customFormat="1" ht="31.5">
       <c r="A9" s="20" t="s">
         <v>4</v>
       </c>
@@ -1883,7 +1984,7 @@
       <c r="AJ9" s="14"/>
       <c r="AK9"/>
     </row>
-    <row r="10" spans="1:38" s="59" customFormat="1" ht="32">
+    <row r="10" spans="1:38" s="59" customFormat="1" ht="31.5">
       <c r="A10" s="20" t="s">
         <v>5</v>
       </c>
@@ -1951,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="85" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="8"/>
@@ -1984,7 +2085,7 @@
       <c r="AI11" s="8"/>
       <c r="AJ11" s="14"/>
     </row>
-    <row r="12" spans="1:38" s="3" customFormat="1" ht="32">
+    <row r="12" spans="1:38" s="3" customFormat="1" ht="31.5">
       <c r="A12" s="20" t="s">
         <v>86</v>
       </c>
@@ -2037,13 +2138,13 @@
     </row>
     <row r="13" spans="1:38" s="3" customFormat="1">
       <c r="A13" s="20" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D13" s="32">
         <v>1</v>
@@ -2052,7 +2153,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="8"/>
@@ -2088,22 +2189,22 @@
     </row>
     <row r="14" spans="1:38" s="3" customFormat="1">
       <c r="A14" s="20" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E14" s="32">
         <v>2</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="8"/>
@@ -2139,13 +2240,13 @@
     </row>
     <row r="15" spans="1:38" s="3" customFormat="1">
       <c r="A15" s="20" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D15" s="32" t="s">
         <v>116</v>
@@ -2154,7 +2255,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="8"/>
@@ -2190,22 +2291,22 @@
     </row>
     <row r="16" spans="1:38" s="3" customFormat="1">
       <c r="A16" s="20" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E16" s="32">
         <v>3</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="8"/>
@@ -2241,22 +2342,22 @@
     </row>
     <row r="17" spans="1:37" s="3" customFormat="1">
       <c r="A17" s="20" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B17" s="48" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E17" s="32">
         <v>3</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="8"/>
@@ -2290,12 +2391,17 @@
       <c r="AJ17" s="14"/>
       <c r="AK17"/>
     </row>
-    <row r="18" spans="1:37" s="3" customFormat="1">
+    <row r="18" spans="1:37">
       <c r="A18" s="20"/>
-      <c r="B18"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="21"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
+      <c r="D18" s="91" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" s="92">
+        <f>SUM(E5:E17)</f>
+        <v>19.5</v>
+      </c>
       <c r="F18" s="62"/>
       <c r="G18" s="12"/>
       <c r="H18" s="8"/>
@@ -2303,18 +2409,18 @@
       <c r="J18" s="15"/>
       <c r="K18" s="8"/>
       <c r="L18" s="45"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="52"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="52"/>
-      <c r="T18" s="53"/>
-      <c r="U18" s="54"/>
-      <c r="V18" s="55"/>
-      <c r="W18" s="53"/>
-      <c r="X18" s="60"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="14"/>
       <c r="Y18" s="12"/>
       <c r="Z18" s="8"/>
       <c r="AA18" s="14"/>
@@ -2327,19 +2433,13 @@
       <c r="AH18" s="12"/>
       <c r="AI18" s="8"/>
       <c r="AJ18" s="14"/>
-      <c r="AK18"/>
     </row>
     <row r="19" spans="1:37">
       <c r="A19" s="20"/>
       <c r="B19" s="48"/>
       <c r="C19" s="21"/>
-      <c r="D19" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="E19" s="25">
-        <f>SUM(E7:E17)</f>
-        <v>18</v>
-      </c>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
       <c r="F19" s="62"/>
       <c r="G19" s="12"/>
       <c r="H19" s="8"/>
@@ -2350,10 +2450,10 @@
       <c r="M19" s="12"/>
       <c r="N19" s="8"/>
       <c r="O19" s="14"/>
-      <c r="P19" s="12"/>
+      <c r="P19" s="15"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="14"/>
-      <c r="S19" s="12"/>
+      <c r="S19" s="15"/>
       <c r="T19" s="8"/>
       <c r="U19" s="14"/>
       <c r="V19" s="15"/>
@@ -2383,8 +2483,8 @@
       <c r="H20" s="8"/>
       <c r="I20" s="14"/>
       <c r="J20" s="15"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="45"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="58"/>
       <c r="M20" s="12"/>
       <c r="N20" s="8"/>
       <c r="O20" s="14"/>
@@ -2411,93 +2511,105 @@
       <c r="AJ20" s="14"/>
     </row>
     <row r="21" spans="1:37">
-      <c r="A21" s="20"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="12"/>
+      <c r="A21" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="15"/>
       <c r="N21" s="8"/>
       <c r="O21" s="14"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="14"/>
-      <c r="Y21" s="12"/>
-      <c r="Z21" s="8"/>
-      <c r="AA21" s="14"/>
-      <c r="AB21" s="12"/>
-      <c r="AC21" s="8"/>
-      <c r="AD21" s="14"/>
-      <c r="AE21" s="15"/>
-      <c r="AF21" s="8"/>
-      <c r="AG21" s="14"/>
-      <c r="AH21" s="12"/>
-      <c r="AI21" s="8"/>
-      <c r="AJ21" s="14"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="41"/>
+      <c r="S21" s="42"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="41"/>
+      <c r="V21" s="42"/>
+      <c r="W21" s="40"/>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="39"/>
+      <c r="Z21" s="40"/>
+      <c r="AA21" s="41"/>
+      <c r="AB21" s="39"/>
+      <c r="AC21" s="40"/>
+      <c r="AD21" s="41"/>
+      <c r="AE21" s="42"/>
+      <c r="AF21" s="40"/>
+      <c r="AG21" s="41"/>
+      <c r="AH21" s="39"/>
+      <c r="AI21" s="40"/>
+      <c r="AJ21" s="41"/>
     </row>
     <row r="22" spans="1:37">
-      <c r="A22" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" s="70" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="71" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="71">
+        <v>0</v>
+      </c>
+      <c r="F22" s="81" t="s">
+        <v>141</v>
+      </c>
       <c r="G22" s="39"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="41"/>
-      <c r="S22" s="42"/>
-      <c r="T22" s="40"/>
-      <c r="U22" s="41"/>
-      <c r="V22" s="42"/>
-      <c r="W22" s="40"/>
-      <c r="X22" s="41"/>
-      <c r="Y22" s="39"/>
-      <c r="Z22" s="40"/>
-      <c r="AA22" s="41"/>
-      <c r="AB22" s="39"/>
-      <c r="AC22" s="40"/>
-      <c r="AD22" s="41"/>
-      <c r="AE22" s="42"/>
-      <c r="AF22" s="40"/>
-      <c r="AG22" s="41"/>
-      <c r="AH22" s="39"/>
-      <c r="AI22" s="40"/>
-      <c r="AJ22" s="41"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="54"/>
+      <c r="P22" s="74"/>
+      <c r="Q22" s="72"/>
+      <c r="R22" s="73"/>
+      <c r="S22" s="74"/>
+      <c r="T22" s="72"/>
+      <c r="U22" s="73"/>
+      <c r="V22" s="74"/>
+      <c r="W22" s="72"/>
+      <c r="X22" s="73"/>
+      <c r="Y22" s="75"/>
+      <c r="Z22" s="72"/>
+      <c r="AA22" s="73"/>
+      <c r="AB22" s="75"/>
+      <c r="AC22" s="72"/>
+      <c r="AD22" s="73"/>
+      <c r="AE22" s="74"/>
+      <c r="AF22" s="72"/>
+      <c r="AG22" s="73"/>
+      <c r="AH22" s="75"/>
+      <c r="AI22" s="72"/>
+      <c r="AJ22" s="73"/>
     </row>
     <row r="23" spans="1:37">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C23" s="70" t="s">
         <v>119</v>
@@ -2509,12 +2621,12 @@
         <v>0</v>
       </c>
       <c r="F23" s="81" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G23" s="39"/>
       <c r="H23" s="72"/>
       <c r="I23" s="73"/>
-      <c r="J23" s="74"/>
+      <c r="J23" s="75"/>
       <c r="K23" s="72"/>
       <c r="L23" s="73"/>
       <c r="M23" s="55"/>
@@ -2543,75 +2655,73 @@
       <c r="AJ23" s="73"/>
     </row>
     <row r="24" spans="1:37">
-      <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" t="s">
-        <v>173</v>
-      </c>
-      <c r="C24" s="70" t="s">
-        <v>119</v>
-      </c>
-      <c r="D24" s="71" t="s">
-        <v>118</v>
-      </c>
-      <c r="E24" s="71">
-        <v>0</v>
-      </c>
-      <c r="F24" s="81" t="s">
-        <v>142</v>
+      <c r="A24" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="32">
+        <v>3</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>64</v>
       </c>
       <c r="G24" s="39"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="73"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="72"/>
-      <c r="L24" s="73"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="54"/>
-      <c r="P24" s="74"/>
-      <c r="Q24" s="72"/>
-      <c r="R24" s="73"/>
-      <c r="S24" s="74"/>
-      <c r="T24" s="72"/>
-      <c r="U24" s="73"/>
-      <c r="V24" s="74"/>
-      <c r="W24" s="72"/>
-      <c r="X24" s="73"/>
-      <c r="Y24" s="75"/>
-      <c r="Z24" s="72"/>
-      <c r="AA24" s="73"/>
-      <c r="AB24" s="75"/>
-      <c r="AC24" s="72"/>
-      <c r="AD24" s="73"/>
-      <c r="AE24" s="74"/>
-      <c r="AF24" s="72"/>
-      <c r="AG24" s="73"/>
-      <c r="AH24" s="75"/>
-      <c r="AI24" s="72"/>
-      <c r="AJ24" s="73"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="53"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="55"/>
+      <c r="T24" s="53"/>
+      <c r="U24" s="54"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="14"/>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="8"/>
+      <c r="AA24" s="14"/>
+      <c r="AB24" s="12"/>
+      <c r="AC24" s="8"/>
+      <c r="AD24" s="14"/>
+      <c r="AE24" s="15"/>
+      <c r="AF24" s="8"/>
+      <c r="AG24" s="14"/>
+      <c r="AH24" s="12"/>
+      <c r="AI24" s="8"/>
+      <c r="AJ24" s="14"/>
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B25" s="48" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D25" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="E25" s="32">
-        <v>2</v>
-      </c>
-      <c r="F25" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="G25" s="39"/>
+      <c r="E25" s="56">
+        <v>6</v>
+      </c>
+      <c r="F25" s="25"/>
+      <c r="G25" s="12"/>
       <c r="H25" s="8"/>
       <c r="I25" s="14"/>
       <c r="J25" s="15"/>
@@ -2620,105 +2730,100 @@
       <c r="M25" s="15"/>
       <c r="N25" s="8"/>
       <c r="O25" s="14"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="53"/>
-      <c r="R25" s="54"/>
-      <c r="S25" s="55"/>
-      <c r="T25" s="53"/>
-      <c r="U25" s="54"/>
-      <c r="V25" s="15"/>
-      <c r="W25" s="8"/>
-      <c r="X25" s="14"/>
-      <c r="Y25" s="12"/>
-      <c r="Z25" s="8"/>
-      <c r="AA25" s="14"/>
-      <c r="AB25" s="12"/>
-      <c r="AC25" s="8"/>
-      <c r="AD25" s="14"/>
-      <c r="AE25" s="15"/>
-      <c r="AF25" s="8"/>
-      <c r="AG25" s="14"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="14"/>
+      <c r="V25" s="55"/>
+      <c r="W25" s="53"/>
+      <c r="X25" s="54"/>
+      <c r="Y25" s="52"/>
+      <c r="Z25" s="53"/>
+      <c r="AA25" s="60"/>
+      <c r="AB25" s="76"/>
+      <c r="AC25" s="77"/>
+      <c r="AD25" s="78"/>
+      <c r="AE25" s="79"/>
+      <c r="AF25" s="77"/>
+      <c r="AG25" s="78"/>
       <c r="AH25" s="12"/>
       <c r="AI25" s="8"/>
       <c r="AJ25" s="14"/>
     </row>
     <row r="26" spans="1:37">
       <c r="A26" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="48" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C26" s="46" t="s">
         <v>121</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="E26" s="86">
-        <v>6</v>
-      </c>
-      <c r="F26" s="25"/>
+        <v>123</v>
+      </c>
+      <c r="E26" s="32">
+        <v>0</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>144</v>
+      </c>
       <c r="G26" s="12"/>
       <c r="H26" s="8"/>
       <c r="I26" s="14"/>
       <c r="J26" s="15"/>
       <c r="K26" s="8"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="15"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="12"/>
       <c r="Q26" s="8"/>
       <c r="R26" s="14"/>
       <c r="S26" s="15"/>
       <c r="T26" s="8"/>
       <c r="U26" s="14"/>
-      <c r="V26" s="55"/>
-      <c r="W26" s="53"/>
-      <c r="X26" s="54"/>
-      <c r="Y26" s="52"/>
-      <c r="Z26" s="53"/>
-      <c r="AA26" s="60"/>
-      <c r="AB26" s="76"/>
-      <c r="AC26" s="77"/>
-      <c r="AD26" s="78"/>
-      <c r="AE26" s="79"/>
-      <c r="AF26" s="77"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="14"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="54"/>
+      <c r="AB26" s="52"/>
+      <c r="AC26" s="53"/>
+      <c r="AD26" s="54"/>
+      <c r="AE26" s="80"/>
+      <c r="AF26" s="8"/>
       <c r="AG26" s="78"/>
-      <c r="AH26" s="12"/>
-      <c r="AI26" s="8"/>
-      <c r="AJ26" s="14"/>
+      <c r="AH26" s="76"/>
+      <c r="AI26" s="77"/>
+      <c r="AJ26" s="78"/>
     </row>
     <row r="27" spans="1:37">
-      <c r="A27" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="C27" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="D27" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="E27" s="32">
-        <v>0</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>146</v>
-      </c>
+      <c r="A27" s="20"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="91" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" s="92">
+        <f>SUM(E22:E26)</f>
+        <v>9</v>
+      </c>
+      <c r="F27" s="62"/>
       <c r="G27" s="12"/>
       <c r="H27" s="8"/>
       <c r="I27" s="14"/>
       <c r="J27" s="15"/>
       <c r="K27" s="8"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="28"/>
-      <c r="P27" s="12"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="15"/>
       <c r="Q27" s="8"/>
       <c r="R27" s="14"/>
       <c r="S27" s="15"/>
@@ -2729,28 +2834,23 @@
       <c r="X27" s="14"/>
       <c r="Y27" s="12"/>
       <c r="Z27" s="8"/>
-      <c r="AA27" s="54"/>
-      <c r="AB27" s="52"/>
-      <c r="AC27" s="53"/>
-      <c r="AD27" s="54"/>
-      <c r="AE27" s="80"/>
+      <c r="AA27" s="14"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="8"/>
+      <c r="AD27" s="14"/>
+      <c r="AE27" s="15"/>
       <c r="AF27" s="8"/>
-      <c r="AG27" s="78"/>
-      <c r="AH27" s="76"/>
-      <c r="AI27" s="77"/>
-      <c r="AJ27" s="78"/>
+      <c r="AG27" s="14"/>
+      <c r="AH27" s="12"/>
+      <c r="AI27" s="8"/>
+      <c r="AJ27" s="14"/>
     </row>
     <row r="28" spans="1:37">
       <c r="A28" s="20"/>
       <c r="B28" s="49"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="E28" s="32">
-        <f>SUM(E23:E27)</f>
-        <v>8</v>
-      </c>
+      <c r="C28" s="46"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
       <c r="F28" s="62"/>
       <c r="G28" s="12"/>
       <c r="H28" s="8"/>
@@ -2786,13 +2886,8 @@
     <row r="29" spans="1:37">
       <c r="A29" s="20"/>
       <c r="B29" s="49"/>
-      <c r="C29" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="D29" s="32">
-        <f>E19+E28</f>
-        <v>26</v>
-      </c>
+      <c r="C29" s="46"/>
+      <c r="D29" s="83"/>
       <c r="E29" s="32"/>
       <c r="F29" s="62"/>
       <c r="G29" s="12"/>
@@ -2827,17 +2922,20 @@
       <c r="AJ29" s="14"/>
     </row>
     <row r="30" spans="1:37">
-      <c r="A30" s="20"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="46" t="s">
-        <v>148</v>
-      </c>
-      <c r="D30" s="83">
-        <f>D29/27</f>
-        <v>0.96296296296296291</v>
-      </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="62"/>
+      <c r="A30" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="25"/>
+      <c r="F30" s="47"/>
       <c r="G30" s="12"/>
       <c r="H30" s="8"/>
       <c r="I30" s="14"/>
@@ -2870,20 +2968,25 @@
       <c r="AJ30" s="14"/>
     </row>
     <row r="31" spans="1:37">
-      <c r="A31" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="50" t="s">
-        <v>54</v>
+      <c r="A31" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="48" t="s">
+        <v>61</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="47"/>
+        <v>66</v>
+      </c>
+      <c r="D31" s="32">
+        <v>2</v>
+      </c>
+      <c r="E31" s="32">
+        <f>D31/4</f>
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="62" t="s">
+        <v>65</v>
+      </c>
       <c r="G31" s="12"/>
       <c r="H31" s="8"/>
       <c r="I31" s="14"/>
@@ -2893,9 +2996,9 @@
       <c r="M31" s="15"/>
       <c r="N31" s="8"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="14"/>
+      <c r="P31" s="55"/>
+      <c r="Q31" s="53"/>
+      <c r="R31" s="60"/>
       <c r="S31" s="15"/>
       <c r="T31" s="8"/>
       <c r="U31" s="14"/>
@@ -2915,26 +3018,21 @@
       <c r="AI31" s="8"/>
       <c r="AJ31" s="14"/>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" ht="31.5">
       <c r="A32" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B32" s="48" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D32" s="32">
         <v>2</v>
       </c>
-      <c r="E32" s="32">
-        <f>D32/4</f>
-        <v>0.5</v>
-      </c>
-      <c r="F32" s="62" t="s">
-        <v>65</v>
-      </c>
+      <c r="E32" s="32"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="12"/>
       <c r="H32" s="8"/>
       <c r="I32" s="14"/>
@@ -2966,20 +3064,21 @@
       <c r="AI32" s="8"/>
       <c r="AJ32" s="14"/>
     </row>
-    <row r="33" spans="1:36" ht="32">
+    <row r="33" spans="1:36" s="1" customFormat="1">
       <c r="A33" s="20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B33" s="48" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="32">
-        <v>2</v>
-      </c>
-      <c r="E33" s="32"/>
+        <v>138</v>
+      </c>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32">
+        <f t="shared" ref="E33:E44" si="0">D33/4</f>
+        <v>0</v>
+      </c>
       <c r="F33" s="62"/>
       <c r="G33" s="12"/>
       <c r="H33" s="8"/>
@@ -2987,9 +3086,9 @@
       <c r="J33" s="15"/>
       <c r="K33" s="8"/>
       <c r="L33" s="14"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="14"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="27"/>
+      <c r="O33" s="28"/>
       <c r="P33" s="55"/>
       <c r="Q33" s="53"/>
       <c r="R33" s="60"/>
@@ -3002,9 +3101,9 @@
       <c r="Y33" s="12"/>
       <c r="Z33" s="8"/>
       <c r="AA33" s="14"/>
-      <c r="AB33" s="12"/>
-      <c r="AC33" s="8"/>
-      <c r="AD33" s="14"/>
+      <c r="AB33" s="34"/>
+      <c r="AC33" s="35"/>
+      <c r="AD33" s="36"/>
       <c r="AE33" s="15"/>
       <c r="AF33" s="8"/>
       <c r="AG33" s="14"/>
@@ -3012,46 +3111,50 @@
       <c r="AI33" s="8"/>
       <c r="AJ33" s="14"/>
     </row>
-    <row r="34" spans="1:36" s="1" customFormat="1">
+    <row r="34" spans="1:36">
       <c r="A34" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B34" s="48" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="D34" s="32"/>
+        <v>67</v>
+      </c>
+      <c r="D34" s="32">
+        <v>4</v>
+      </c>
       <c r="E34" s="32">
-        <f t="shared" ref="E34:E45" si="0">D34/4</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="62"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F34" s="62" t="s">
+        <v>139</v>
+      </c>
       <c r="G34" s="12"/>
       <c r="H34" s="8"/>
       <c r="I34" s="14"/>
       <c r="J34" s="15"/>
       <c r="K34" s="8"/>
       <c r="L34" s="14"/>
-      <c r="M34" s="29"/>
-      <c r="N34" s="27"/>
-      <c r="O34" s="28"/>
-      <c r="P34" s="55"/>
-      <c r="Q34" s="53"/>
-      <c r="R34" s="60"/>
-      <c r="S34" s="15"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="14"/>
-      <c r="V34" s="15"/>
-      <c r="W34" s="8"/>
-      <c r="X34" s="14"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="55"/>
+      <c r="T34" s="53"/>
+      <c r="U34" s="54"/>
+      <c r="V34" s="55"/>
+      <c r="W34" s="53"/>
+      <c r="X34" s="54"/>
       <c r="Y34" s="12"/>
       <c r="Z34" s="8"/>
       <c r="AA34" s="14"/>
-      <c r="AB34" s="34"/>
-      <c r="AC34" s="35"/>
-      <c r="AD34" s="36"/>
+      <c r="AB34" s="12"/>
+      <c r="AC34" s="8"/>
+      <c r="AD34" s="14"/>
       <c r="AE34" s="15"/>
       <c r="AF34" s="8"/>
       <c r="AG34" s="14"/>
@@ -3061,24 +3164,22 @@
     </row>
     <row r="35" spans="1:36">
       <c r="A35" s="20" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B35" s="48" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D35" s="32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E35" s="32">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F35" s="62" t="s">
-        <v>139</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="F35" s="62"/>
       <c r="G35" s="12"/>
       <c r="H35" s="8"/>
       <c r="I35" s="14"/>
@@ -3091,14 +3192,13 @@
       <c r="P35" s="15"/>
       <c r="Q35" s="8"/>
       <c r="R35" s="14"/>
-      <c r="S35" s="55"/>
-      <c r="T35" s="53"/>
-      <c r="U35" s="54"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="14"/>
       <c r="V35" s="55"/>
       <c r="W35" s="53"/>
-      <c r="X35" s="54"/>
+      <c r="X35" s="14"/>
       <c r="Y35" s="12"/>
-      <c r="Z35" s="8"/>
       <c r="AA35" s="14"/>
       <c r="AB35" s="12"/>
       <c r="AC35" s="8"/>
@@ -3112,13 +3212,13 @@
     </row>
     <row r="36" spans="1:36">
       <c r="A36" s="20" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B36" s="48" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D36" s="32">
         <v>2</v>
@@ -3134,9 +3234,9 @@
       <c r="J36" s="15"/>
       <c r="K36" s="8"/>
       <c r="L36" s="14"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="14"/>
+      <c r="M36" s="37"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="36"/>
       <c r="P36" s="15"/>
       <c r="Q36" s="8"/>
       <c r="R36" s="14"/>
@@ -3160,20 +3260,20 @@
     </row>
     <row r="37" spans="1:36">
       <c r="A37" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B37" s="48" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D37" s="32">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E37" s="32">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F37" s="62"/>
       <c r="G37" s="12"/>
@@ -3182,18 +3282,18 @@
       <c r="J37" s="15"/>
       <c r="K37" s="8"/>
       <c r="L37" s="14"/>
-      <c r="M37" s="37"/>
-      <c r="N37" s="35"/>
-      <c r="O37" s="36"/>
-      <c r="P37" s="15"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="12"/>
       <c r="Q37" s="8"/>
       <c r="R37" s="14"/>
-      <c r="S37" s="15"/>
+      <c r="S37" s="12"/>
       <c r="T37" s="8"/>
       <c r="U37" s="14"/>
       <c r="V37" s="55"/>
       <c r="W37" s="53"/>
-      <c r="X37" s="14"/>
+      <c r="X37" s="60"/>
       <c r="Y37" s="12"/>
       <c r="AA37" s="14"/>
       <c r="AB37" s="12"/>
@@ -3206,15 +3306,15 @@
       <c r="AI37" s="8"/>
       <c r="AJ37" s="14"/>
     </row>
-    <row r="38" spans="1:36">
+    <row r="38" spans="1:36" s="1" customFormat="1">
       <c r="A38" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B38" s="48" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D38" s="32">
         <v>6</v>
@@ -3227,7 +3327,7 @@
       <c r="G38" s="12"/>
       <c r="H38" s="8"/>
       <c r="I38" s="14"/>
-      <c r="J38" s="15"/>
+      <c r="J38" s="12"/>
       <c r="K38" s="8"/>
       <c r="L38" s="14"/>
       <c r="M38" s="12"/>
@@ -3239,13 +3339,14 @@
       <c r="S38" s="12"/>
       <c r="T38" s="8"/>
       <c r="U38" s="14"/>
-      <c r="V38" s="55"/>
-      <c r="W38" s="53"/>
-      <c r="X38" s="60"/>
-      <c r="Y38" s="12"/>
-      <c r="AA38" s="14"/>
-      <c r="AB38" s="12"/>
-      <c r="AC38" s="8"/>
+      <c r="V38" s="12"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="14"/>
+      <c r="Y38" s="53"/>
+      <c r="Z38" s="53"/>
+      <c r="AA38" s="54"/>
+      <c r="AB38" s="52"/>
+      <c r="AC38" s="53"/>
       <c r="AD38" s="14"/>
       <c r="AE38" s="15"/>
       <c r="AF38" s="8"/>
@@ -3254,22 +3355,22 @@
       <c r="AI38" s="8"/>
       <c r="AJ38" s="14"/>
     </row>
-    <row r="39" spans="1:36" s="1" customFormat="1">
+    <row r="39" spans="1:36">
       <c r="A39" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B39" s="48" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D39" s="32">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E39" s="32">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="F39" s="62"/>
       <c r="G39" s="12"/>
@@ -3290,14 +3391,14 @@
       <c r="V39" s="12"/>
       <c r="W39" s="8"/>
       <c r="X39" s="14"/>
-      <c r="Y39" s="53"/>
-      <c r="Z39" s="53"/>
-      <c r="AA39" s="54"/>
-      <c r="AB39" s="52"/>
-      <c r="AC39" s="53"/>
-      <c r="AD39" s="14"/>
-      <c r="AE39" s="15"/>
-      <c r="AF39" s="8"/>
+      <c r="Y39" s="15"/>
+      <c r="Z39" s="8"/>
+      <c r="AA39" s="14"/>
+      <c r="AB39" s="34"/>
+      <c r="AC39" s="35"/>
+      <c r="AD39" s="54"/>
+      <c r="AE39" s="55"/>
+      <c r="AF39" s="53"/>
       <c r="AG39" s="14"/>
       <c r="AH39" s="12"/>
       <c r="AI39" s="8"/>
@@ -3305,62 +3406,62 @@
     </row>
     <row r="40" spans="1:36">
       <c r="A40" s="20" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B40" s="48" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D40" s="32">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E40" s="32">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="F40" s="62"/>
       <c r="G40" s="12"/>
       <c r="H40" s="8"/>
       <c r="I40" s="14"/>
-      <c r="J40" s="12"/>
+      <c r="J40" s="15"/>
       <c r="K40" s="8"/>
       <c r="L40" s="14"/>
       <c r="M40" s="12"/>
       <c r="N40" s="8"/>
       <c r="O40" s="14"/>
-      <c r="P40" s="12"/>
+      <c r="P40" s="15"/>
       <c r="Q40" s="8"/>
       <c r="R40" s="14"/>
-      <c r="S40" s="12"/>
+      <c r="S40" s="15"/>
       <c r="T40" s="8"/>
       <c r="U40" s="14"/>
-      <c r="V40" s="12"/>
+      <c r="V40" s="15"/>
       <c r="W40" s="8"/>
       <c r="X40" s="14"/>
       <c r="Y40" s="15"/>
       <c r="Z40" s="8"/>
       <c r="AA40" s="14"/>
-      <c r="AB40" s="34"/>
-      <c r="AC40" s="35"/>
-      <c r="AD40" s="54"/>
+      <c r="AB40" s="15"/>
+      <c r="AC40" s="8"/>
+      <c r="AD40" s="14"/>
       <c r="AE40" s="55"/>
       <c r="AF40" s="53"/>
-      <c r="AG40" s="14"/>
+      <c r="AG40" s="54"/>
       <c r="AH40" s="12"/>
       <c r="AI40" s="8"/>
       <c r="AJ40" s="14"/>
     </row>
     <row r="41" spans="1:36">
       <c r="A41" s="20" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B41" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D41" s="32">
         <v>2</v>
@@ -3369,14 +3470,14 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F41" s="62"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="12"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="15"/>
       <c r="N41" s="8"/>
       <c r="O41" s="14"/>
       <c r="P41" s="15"/>
@@ -3391,40 +3492,40 @@
       <c r="Y41" s="15"/>
       <c r="Z41" s="8"/>
       <c r="AA41" s="14"/>
-      <c r="AB41" s="15"/>
+      <c r="AB41" s="12"/>
       <c r="AC41" s="8"/>
       <c r="AD41" s="14"/>
       <c r="AE41" s="55"/>
       <c r="AF41" s="53"/>
       <c r="AG41" s="54"/>
-      <c r="AH41" s="12"/>
-      <c r="AI41" s="8"/>
-      <c r="AJ41" s="14"/>
+      <c r="AH41" s="26"/>
+      <c r="AI41" s="27"/>
+      <c r="AJ41" s="28"/>
     </row>
     <row r="42" spans="1:36">
       <c r="A42" s="20" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B42" s="48" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D42" s="32">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E42" s="32">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="F42" s="47"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="28"/>
+        <v>2</v>
+      </c>
+      <c r="F42" s="62"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="14"/>
       <c r="M42" s="15"/>
       <c r="N42" s="8"/>
       <c r="O42" s="14"/>
@@ -3443,31 +3544,31 @@
       <c r="AB42" s="12"/>
       <c r="AC42" s="8"/>
       <c r="AD42" s="14"/>
-      <c r="AE42" s="55"/>
-      <c r="AF42" s="53"/>
+      <c r="AE42" s="15"/>
+      <c r="AF42" s="8"/>
       <c r="AG42" s="54"/>
-      <c r="AH42" s="26"/>
-      <c r="AI42" s="27"/>
-      <c r="AJ42" s="28"/>
+      <c r="AH42" s="52"/>
+      <c r="AI42" s="61"/>
+      <c r="AJ42" s="14"/>
     </row>
     <row r="43" spans="1:36">
       <c r="A43" s="20" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
       <c r="B43" s="48" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D43" s="32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E43" s="32">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F43" s="62"/>
+        <v>1.5</v>
+      </c>
+      <c r="F43" s="47"/>
       <c r="G43" s="12"/>
       <c r="H43" s="8"/>
       <c r="I43" s="14"/>
@@ -3477,16 +3578,16 @@
       <c r="M43" s="15"/>
       <c r="N43" s="8"/>
       <c r="O43" s="14"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="8"/>
-      <c r="U43" s="14"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="8"/>
-      <c r="X43" s="14"/>
-      <c r="Y43" s="15"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="27"/>
+      <c r="R43" s="28"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="27"/>
+      <c r="U43" s="28"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="27"/>
+      <c r="X43" s="28"/>
+      <c r="Y43" s="12"/>
       <c r="Z43" s="8"/>
       <c r="AA43" s="14"/>
       <c r="AB43" s="12"/>
@@ -3494,47 +3595,47 @@
       <c r="AD43" s="14"/>
       <c r="AE43" s="15"/>
       <c r="AF43" s="8"/>
-      <c r="AG43" s="54"/>
-      <c r="AH43" s="52"/>
-      <c r="AI43" s="61"/>
-      <c r="AJ43" s="14"/>
+      <c r="AG43" s="14"/>
+      <c r="AH43" s="12"/>
+      <c r="AI43" s="53"/>
+      <c r="AJ43" s="54"/>
     </row>
     <row r="44" spans="1:36">
       <c r="A44" s="20" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B44" s="48" t="s">
-        <v>74</v>
+        <v>135</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D44" s="32">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E44" s="32">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="F44" s="47"/>
+        <v>2</v>
+      </c>
+      <c r="F44" s="62"/>
       <c r="G44" s="12"/>
       <c r="H44" s="8"/>
       <c r="I44" s="14"/>
       <c r="J44" s="15"/>
       <c r="K44" s="8"/>
       <c r="L44" s="14"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="27"/>
-      <c r="R44" s="28"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="27"/>
-      <c r="U44" s="28"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="27"/>
-      <c r="X44" s="28"/>
+      <c r="M44" s="55"/>
+      <c r="N44" s="53"/>
+      <c r="O44" s="60"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="8"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="8"/>
+      <c r="X44" s="14"/>
       <c r="Y44" s="12"/>
       <c r="Z44" s="8"/>
       <c r="AA44" s="14"/>
@@ -3545,36 +3646,30 @@
       <c r="AF44" s="8"/>
       <c r="AG44" s="14"/>
       <c r="AH44" s="12"/>
-      <c r="AI44" s="53"/>
-      <c r="AJ44" s="54"/>
-    </row>
-    <row r="45" spans="1:36">
-      <c r="A45" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="B45" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="32">
-        <v>8</v>
-      </c>
-      <c r="E45" s="32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F45" s="62"/>
+      <c r="AI44" s="8"/>
+      <c r="AJ44" s="14"/>
+    </row>
+    <row r="45" spans="1:36" s="38" customFormat="1">
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="91" t="s">
+        <v>171</v>
+      </c>
+      <c r="E45" s="92">
+        <f>SUM(E31:E44)</f>
+        <v>14.5</v>
+      </c>
+      <c r="F45" s="47"/>
       <c r="G45" s="12"/>
       <c r="H45" s="8"/>
       <c r="I45" s="14"/>
       <c r="J45" s="15"/>
       <c r="K45" s="8"/>
       <c r="L45" s="14"/>
-      <c r="M45" s="55"/>
-      <c r="N45" s="53"/>
-      <c r="O45" s="60"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="14"/>
       <c r="P45" s="15"/>
       <c r="Q45" s="8"/>
       <c r="R45" s="14"/>
@@ -3590,9 +3685,9 @@
       <c r="AB45" s="12"/>
       <c r="AC45" s="8"/>
       <c r="AD45" s="14"/>
-      <c r="AE45" s="15"/>
-      <c r="AF45" s="8"/>
-      <c r="AG45" s="14"/>
+      <c r="AE45" s="29"/>
+      <c r="AF45" s="27"/>
+      <c r="AG45" s="28"/>
       <c r="AH45" s="12"/>
       <c r="AI45" s="8"/>
       <c r="AJ45" s="14"/>
@@ -3601,13 +3696,8 @@
       <c r="A46" s="20"/>
       <c r="B46" s="20"/>
       <c r="C46" s="21"/>
-      <c r="D46" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="E46" s="25">
-        <f>SUM(E32:E45)</f>
-        <v>14.5</v>
-      </c>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
       <c r="F46" s="47"/>
       <c r="G46" s="12"/>
       <c r="H46" s="8"/>
@@ -3640,16 +3730,19 @@
       <c r="AI46" s="8"/>
       <c r="AJ46" s="14"/>
     </row>
-    <row r="47" spans="1:36">
-      <c r="A47" s="20"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="50">
-        <f>E46+E28+E19</f>
-        <v>40.5</v>
-      </c>
+    <row r="47" spans="1:36" s="38" customFormat="1">
+      <c r="A47" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="B47" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
       <c r="G47" s="12"/>
       <c r="H47" s="8"/>
       <c r="I47" s="14"/>
@@ -3671,76 +3764,85 @@
       <c r="Y47" s="12"/>
       <c r="Z47" s="8"/>
       <c r="AA47" s="14"/>
-      <c r="AB47" s="34"/>
-      <c r="AC47" s="35"/>
-      <c r="AD47" s="36"/>
-      <c r="AE47" s="15"/>
-      <c r="AF47" s="8"/>
-      <c r="AG47" s="14"/>
+      <c r="AB47" s="12"/>
+      <c r="AC47" s="8"/>
+      <c r="AD47" s="14"/>
+      <c r="AE47" s="29"/>
+      <c r="AF47" s="27"/>
+      <c r="AG47" s="28"/>
       <c r="AH47" s="12"/>
       <c r="AI47" s="8"/>
       <c r="AJ47" s="14"/>
     </row>
-    <row r="48" spans="1:36">
-      <c r="A48" s="33"/>
-      <c r="B48" s="69" t="s">
-        <v>140</v>
-      </c>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="E48" s="32">
-        <f>F47/27</f>
-        <v>1.5</v>
-      </c>
-      <c r="F48" s="62"/>
-      <c r="G48" s="34"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="36"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="35"/>
-      <c r="L48" s="36"/>
+    <row r="48" spans="1:36" s="38" customFormat="1">
+      <c r="A48" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="B48" s="86" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" s="86" t="s">
+        <v>182</v>
+      </c>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56">
+        <v>0.25</v>
+      </c>
+      <c r="F48" s="56"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="14"/>
       <c r="M48" s="15"/>
       <c r="N48" s="8"/>
       <c r="O48" s="14"/>
       <c r="P48" s="15"/>
       <c r="Q48" s="8"/>
       <c r="R48" s="14"/>
-      <c r="S48" s="15"/>
+      <c r="S48" s="55"/>
       <c r="T48" s="8"/>
       <c r="U48" s="14"/>
       <c r="V48" s="15"/>
       <c r="W48" s="8"/>
       <c r="X48" s="14"/>
-      <c r="Y48" s="34"/>
-      <c r="Z48" s="35"/>
-      <c r="AA48" s="36"/>
+      <c r="Y48" s="12"/>
+      <c r="Z48" s="8"/>
+      <c r="AA48" s="14"/>
       <c r="AB48" s="12"/>
       <c r="AC48" s="8"/>
       <c r="AD48" s="14"/>
-      <c r="AE48" s="15"/>
-      <c r="AF48" s="8"/>
-      <c r="AG48" s="14"/>
-      <c r="AH48" s="34"/>
-      <c r="AI48" s="35"/>
-      <c r="AJ48" s="36"/>
-    </row>
-    <row r="49" spans="1:36" ht="32">
-      <c r="A49" s="33"/>
-      <c r="B49" s="82" t="s">
-        <v>143</v>
-      </c>
-      <c r="C49" s="32"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="29"/>
-      <c r="K49" s="27"/>
-      <c r="L49" s="28"/>
+      <c r="AE48" s="29"/>
+      <c r="AF48" s="27"/>
+      <c r="AG48" s="28"/>
+      <c r="AH48" s="12"/>
+      <c r="AI48" s="8"/>
+      <c r="AJ48" s="14"/>
+    </row>
+    <row r="49" spans="1:36" s="38" customFormat="1">
+      <c r="A49" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="B49" s="86" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" s="86" t="s">
+        <v>182</v>
+      </c>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56">
+        <v>1.5</v>
+      </c>
+      <c r="F49" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="G49" s="12"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="14"/>
       <c r="M49" s="15"/>
       <c r="N49" s="8"/>
       <c r="O49" s="14"/>
@@ -3748,31 +3850,39 @@
       <c r="Q49" s="8"/>
       <c r="R49" s="14"/>
       <c r="S49" s="15"/>
-      <c r="T49" s="8"/>
-      <c r="U49" s="14"/>
-      <c r="V49" s="15"/>
-      <c r="W49" s="8"/>
+      <c r="T49" s="53"/>
+      <c r="U49" s="54"/>
+      <c r="V49" s="55"/>
+      <c r="W49" s="53"/>
       <c r="X49" s="14"/>
-      <c r="Y49" s="26"/>
-      <c r="Z49" s="27"/>
-      <c r="AA49" s="28"/>
-      <c r="AB49" s="15"/>
+      <c r="Y49" s="12"/>
+      <c r="Z49" s="8"/>
+      <c r="AA49" s="14"/>
+      <c r="AB49" s="12"/>
       <c r="AC49" s="8"/>
       <c r="AD49" s="14"/>
-      <c r="AE49" s="15"/>
-      <c r="AF49" s="8"/>
-      <c r="AG49" s="14"/>
-      <c r="AH49" s="34"/>
-      <c r="AI49" s="35"/>
-      <c r="AJ49" s="36"/>
-    </row>
-    <row r="50" spans="1:36">
-      <c r="A50" s="33"/>
-      <c r="B50" s="48"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="64"/>
+      <c r="AE49" s="29"/>
+      <c r="AF49" s="27"/>
+      <c r="AG49" s="28"/>
+      <c r="AH49" s="12"/>
+      <c r="AI49" s="8"/>
+      <c r="AJ49" s="14"/>
+    </row>
+    <row r="50" spans="1:36" s="38" customFormat="1">
+      <c r="A50" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" s="86" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" s="86" t="s">
+        <v>182</v>
+      </c>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56">
+        <v>1</v>
+      </c>
+      <c r="F50" s="56"/>
       <c r="G50" s="12"/>
       <c r="H50" s="8"/>
       <c r="I50" s="14"/>
@@ -3789,28 +3899,36 @@
       <c r="T50" s="8"/>
       <c r="U50" s="14"/>
       <c r="V50" s="15"/>
-      <c r="W50" s="8"/>
-      <c r="X50" s="14"/>
-      <c r="Y50" s="12"/>
+      <c r="W50" s="53"/>
+      <c r="X50" s="54"/>
+      <c r="Y50" s="52"/>
       <c r="Z50" s="8"/>
       <c r="AA50" s="14"/>
-      <c r="AB50" s="15"/>
+      <c r="AB50" s="12"/>
       <c r="AC50" s="8"/>
       <c r="AD50" s="14"/>
-      <c r="AE50" s="15"/>
-      <c r="AF50" s="8"/>
-      <c r="AG50" s="14"/>
+      <c r="AE50" s="29"/>
+      <c r="AF50" s="27"/>
+      <c r="AG50" s="28"/>
       <c r="AH50" s="12"/>
       <c r="AI50" s="8"/>
       <c r="AJ50" s="14"/>
     </row>
-    <row r="51" spans="1:36" s="23" customFormat="1">
-      <c r="A51" s="20"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="64"/>
+    <row r="51" spans="1:36" s="38" customFormat="1">
+      <c r="A51" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B51" s="86" t="s">
+        <v>179</v>
+      </c>
+      <c r="C51" s="86" t="s">
+        <v>182</v>
+      </c>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56">
+        <v>1</v>
+      </c>
+      <c r="F51" s="56"/>
       <c r="G51" s="12"/>
       <c r="H51" s="8"/>
       <c r="I51" s="14"/>
@@ -3830,25 +3948,30 @@
       <c r="W51" s="8"/>
       <c r="X51" s="14"/>
       <c r="Y51" s="12"/>
-      <c r="Z51" s="8"/>
-      <c r="AA51" s="14"/>
-      <c r="AB51" s="15"/>
-      <c r="AC51" s="8"/>
+      <c r="Z51" s="53"/>
+      <c r="AA51" s="54"/>
+      <c r="AB51" s="52"/>
+      <c r="AC51" s="53"/>
       <c r="AD51" s="14"/>
-      <c r="AE51" s="15"/>
-      <c r="AF51" s="8"/>
-      <c r="AG51" s="14"/>
-      <c r="AH51" s="15"/>
+      <c r="AE51" s="29"/>
+      <c r="AF51" s="27"/>
+      <c r="AG51" s="28"/>
+      <c r="AH51" s="12"/>
       <c r="AI51" s="8"/>
       <c r="AJ51" s="14"/>
     </row>
-    <row r="52" spans="1:36">
-      <c r="A52" s="20"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="65"/>
+    <row r="52" spans="1:36" s="38" customFormat="1">
+      <c r="A52" s="24"/>
+      <c r="B52" s="86"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="91" t="s">
+        <v>171</v>
+      </c>
+      <c r="E52" s="92">
+        <f>SUM(E48:E51)</f>
+        <v>3.75</v>
+      </c>
+      <c r="F52" s="56"/>
       <c r="G52" s="12"/>
       <c r="H52" s="8"/>
       <c r="I52" s="14"/>
@@ -3870,32 +3993,29 @@
       <c r="Y52" s="12"/>
       <c r="Z52" s="8"/>
       <c r="AA52" s="14"/>
-      <c r="AB52" s="15"/>
+      <c r="AB52" s="12"/>
       <c r="AC52" s="8"/>
       <c r="AD52" s="14"/>
-      <c r="AE52" s="15"/>
-      <c r="AF52" s="8"/>
-      <c r="AG52" s="14"/>
-      <c r="AH52" s="15"/>
+      <c r="AE52" s="29"/>
+      <c r="AF52" s="27"/>
+      <c r="AG52" s="28"/>
+      <c r="AH52" s="12"/>
       <c r="AI52" s="8"/>
       <c r="AJ52" s="14"/>
     </row>
-    <row r="53" spans="1:36">
+    <row r="53" spans="1:36" ht="16.5" thickBot="1">
       <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="65"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="56"/>
       <c r="G53" s="12"/>
       <c r="H53" s="8"/>
       <c r="I53" s="14"/>
       <c r="J53" s="15"/>
       <c r="K53" s="8"/>
       <c r="L53" s="14"/>
-      <c r="M53" s="37"/>
-      <c r="N53" s="35"/>
-      <c r="O53" s="36"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="14"/>
       <c r="P53" s="15"/>
       <c r="Q53" s="8"/>
       <c r="R53" s="14"/>
@@ -3908,68 +4028,76 @@
       <c r="Y53" s="12"/>
       <c r="Z53" s="8"/>
       <c r="AA53" s="14"/>
-      <c r="AB53" s="15"/>
-      <c r="AC53" s="8"/>
-      <c r="AD53" s="14"/>
+      <c r="AB53" s="34"/>
+      <c r="AC53" s="35"/>
+      <c r="AD53" s="36"/>
       <c r="AE53" s="15"/>
       <c r="AF53" s="8"/>
       <c r="AG53" s="14"/>
-      <c r="AH53" s="15"/>
+      <c r="AH53" s="12"/>
       <c r="AI53" s="8"/>
       <c r="AJ53" s="14"/>
     </row>
     <row r="54" spans="1:36">
-      <c r="A54" s="23"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="65"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="28"/>
-      <c r="J54" s="29"/>
-      <c r="K54" s="27"/>
-      <c r="L54" s="28"/>
-      <c r="M54" s="29"/>
-      <c r="N54" s="27"/>
-      <c r="O54" s="28"/>
-      <c r="P54" s="29"/>
-      <c r="Q54" s="27"/>
-      <c r="R54" s="28"/>
-      <c r="S54" s="29"/>
-      <c r="T54" s="27"/>
-      <c r="U54" s="28"/>
-      <c r="V54" s="29"/>
-      <c r="W54" s="27"/>
-      <c r="X54" s="28"/>
-      <c r="Y54" s="26"/>
-      <c r="Z54" s="27"/>
-      <c r="AA54" s="28"/>
-      <c r="AB54" s="29"/>
-      <c r="AC54" s="27"/>
-      <c r="AD54" s="28"/>
-      <c r="AE54" s="29"/>
-      <c r="AF54" s="27"/>
-      <c r="AG54" s="28"/>
-      <c r="AH54" s="15"/>
-      <c r="AI54" s="8"/>
-      <c r="AJ54" s="14"/>
-    </row>
-    <row r="55" spans="1:36">
-      <c r="A55" s="20"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="65"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="15"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="12"/>
+      <c r="A54" s="33"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="87" t="s">
+        <v>185</v>
+      </c>
+      <c r="E54" s="88">
+        <f>E45+E27+E18+E52</f>
+        <v>46.75</v>
+      </c>
+      <c r="F54" s="62"/>
+      <c r="G54" s="34"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="36"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="35"/>
+      <c r="L54" s="36"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="8"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="15"/>
+      <c r="T54" s="8"/>
+      <c r="U54" s="14"/>
+      <c r="V54" s="15"/>
+      <c r="W54" s="8"/>
+      <c r="X54" s="14"/>
+      <c r="Y54" s="34"/>
+      <c r="Z54" s="35"/>
+      <c r="AA54" s="36"/>
+      <c r="AB54" s="12"/>
+      <c r="AC54" s="8"/>
+      <c r="AD54" s="14"/>
+      <c r="AE54" s="15"/>
+      <c r="AF54" s="8"/>
+      <c r="AG54" s="14"/>
+      <c r="AH54" s="34"/>
+      <c r="AI54" s="35"/>
+      <c r="AJ54" s="36"/>
+    </row>
+    <row r="55" spans="1:36" ht="16.5" thickBot="1">
+      <c r="A55" s="33"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="89" t="s">
+        <v>186</v>
+      </c>
+      <c r="E55" s="90">
+        <f>E54/27</f>
+        <v>1.7314814814814814</v>
+      </c>
+      <c r="F55" s="47"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="28"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="27"/>
+      <c r="L55" s="28"/>
+      <c r="M55" s="15"/>
       <c r="N55" s="8"/>
       <c r="O55" s="14"/>
       <c r="P55" s="15"/>
@@ -3981,33 +4109,33 @@
       <c r="V55" s="15"/>
       <c r="W55" s="8"/>
       <c r="X55" s="14"/>
-      <c r="Y55" s="12"/>
-      <c r="Z55" s="8"/>
-      <c r="AA55" s="14"/>
+      <c r="Y55" s="26"/>
+      <c r="Z55" s="27"/>
+      <c r="AA55" s="28"/>
       <c r="AB55" s="15"/>
       <c r="AC55" s="8"/>
       <c r="AD55" s="14"/>
       <c r="AE55" s="15"/>
       <c r="AF55" s="8"/>
       <c r="AG55" s="14"/>
-      <c r="AH55" s="15"/>
-      <c r="AI55" s="8"/>
-      <c r="AJ55" s="14"/>
+      <c r="AH55" s="34"/>
+      <c r="AI55" s="35"/>
+      <c r="AJ55" s="36"/>
     </row>
     <row r="56" spans="1:36">
-      <c r="A56" s="20"/>
-      <c r="B56" s="31"/>
+      <c r="A56" s="33"/>
+      <c r="B56" s="48"/>
       <c r="C56" s="21"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="65"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="64"/>
       <c r="G56" s="12"/>
       <c r="H56" s="8"/>
       <c r="I56" s="14"/>
       <c r="J56" s="15"/>
       <c r="K56" s="8"/>
       <c r="L56" s="14"/>
-      <c r="M56" s="12"/>
+      <c r="M56" s="15"/>
       <c r="N56" s="8"/>
       <c r="O56" s="14"/>
       <c r="P56" s="15"/>
@@ -4028,24 +4156,26 @@
       <c r="AE56" s="15"/>
       <c r="AF56" s="8"/>
       <c r="AG56" s="14"/>
-      <c r="AH56" s="29"/>
-      <c r="AI56" s="27"/>
-      <c r="AJ56" s="28"/>
-    </row>
-    <row r="57" spans="1:36" s="1" customFormat="1">
+      <c r="AH56" s="12"/>
+      <c r="AI56" s="8"/>
+      <c r="AJ56" s="14"/>
+    </row>
+    <row r="57" spans="1:36" s="23" customFormat="1">
       <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
+      <c r="B57" s="69" t="s">
+        <v>140</v>
+      </c>
       <c r="C57" s="21"/>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="65"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="64"/>
       <c r="G57" s="12"/>
       <c r="H57" s="8"/>
       <c r="I57" s="14"/>
       <c r="J57" s="15"/>
       <c r="K57" s="8"/>
       <c r="L57" s="14"/>
-      <c r="M57" s="12"/>
+      <c r="M57" s="15"/>
       <c r="N57" s="8"/>
       <c r="O57" s="14"/>
       <c r="P57" s="15"/>
@@ -4070,9 +4200,11 @@
       <c r="AI57" s="8"/>
       <c r="AJ57" s="14"/>
     </row>
-    <row r="58" spans="1:36">
+    <row r="58" spans="1:36" ht="31.5">
       <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
+      <c r="B58" s="82" t="s">
+        <v>143</v>
+      </c>
       <c r="C58" s="21"/>
       <c r="D58" s="22"/>
       <c r="E58" s="22"/>
@@ -4083,7 +4215,7 @@
       <c r="J58" s="15"/>
       <c r="K58" s="8"/>
       <c r="L58" s="14"/>
-      <c r="M58" s="12"/>
+      <c r="M58" s="15"/>
       <c r="N58" s="8"/>
       <c r="O58" s="14"/>
       <c r="P58" s="15"/>
@@ -4110,20 +4242,20 @@
     </row>
     <row r="59" spans="1:36">
       <c r="A59" s="20"/>
-      <c r="B59" s="23"/>
+      <c r="B59" s="20"/>
       <c r="C59" s="21"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="64"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="65"/>
       <c r="G59" s="12"/>
       <c r="H59" s="8"/>
       <c r="I59" s="14"/>
       <c r="J59" s="15"/>
       <c r="K59" s="8"/>
       <c r="L59" s="14"/>
-      <c r="M59" s="12"/>
-      <c r="N59" s="8"/>
-      <c r="O59" s="14"/>
+      <c r="M59" s="37"/>
+      <c r="N59" s="35"/>
+      <c r="O59" s="36"/>
       <c r="P59" s="15"/>
       <c r="Q59" s="8"/>
       <c r="R59" s="14"/>
@@ -4148,7 +4280,6 @@
     </row>
     <row r="60" spans="1:36">
       <c r="A60" s="23"/>
-      <c r="B60" s="23"/>
       <c r="C60" s="25"/>
       <c r="D60" s="22"/>
       <c r="E60" s="22"/>
@@ -4159,7 +4290,7 @@
       <c r="J60" s="29"/>
       <c r="K60" s="27"/>
       <c r="L60" s="28"/>
-      <c r="M60" s="26"/>
+      <c r="M60" s="29"/>
       <c r="N60" s="27"/>
       <c r="O60" s="28"/>
       <c r="P60" s="29"/>
@@ -4174,9 +4305,9 @@
       <c r="Y60" s="26"/>
       <c r="Z60" s="27"/>
       <c r="AA60" s="28"/>
-      <c r="AB60" s="15"/>
-      <c r="AC60" s="8"/>
-      <c r="AD60" s="14"/>
+      <c r="AB60" s="29"/>
+      <c r="AC60" s="27"/>
+      <c r="AD60" s="28"/>
       <c r="AE60" s="29"/>
       <c r="AF60" s="27"/>
       <c r="AG60" s="28"/>
@@ -4186,11 +4317,10 @@
     </row>
     <row r="61" spans="1:36">
       <c r="A61" s="20"/>
-      <c r="B61" s="31"/>
       <c r="C61" s="21"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="64"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="65"/>
       <c r="G61" s="12"/>
       <c r="H61" s="8"/>
       <c r="I61" s="14"/>
@@ -4212,7 +4342,7 @@
       <c r="Y61" s="12"/>
       <c r="Z61" s="8"/>
       <c r="AA61" s="14"/>
-      <c r="AB61" s="12"/>
+      <c r="AB61" s="15"/>
       <c r="AC61" s="8"/>
       <c r="AD61" s="14"/>
       <c r="AE61" s="15"/>
@@ -4250,23 +4380,23 @@
       <c r="Y62" s="12"/>
       <c r="Z62" s="8"/>
       <c r="AA62" s="14"/>
-      <c r="AB62" s="12"/>
+      <c r="AB62" s="15"/>
       <c r="AC62" s="8"/>
       <c r="AD62" s="14"/>
       <c r="AE62" s="15"/>
       <c r="AF62" s="8"/>
       <c r="AG62" s="14"/>
-      <c r="AH62" s="15"/>
-      <c r="AI62" s="8"/>
-      <c r="AJ62" s="14"/>
-    </row>
-    <row r="63" spans="1:36">
+      <c r="AH62" s="29"/>
+      <c r="AI62" s="27"/>
+      <c r="AJ62" s="28"/>
+    </row>
+    <row r="63" spans="1:36" s="1" customFormat="1">
       <c r="A63" s="20"/>
-      <c r="B63" s="31"/>
+      <c r="B63" s="20"/>
       <c r="C63" s="21"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="64"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="65"/>
       <c r="G63" s="12"/>
       <c r="H63" s="8"/>
       <c r="I63" s="14"/>
@@ -4288,19 +4418,19 @@
       <c r="Y63" s="12"/>
       <c r="Z63" s="8"/>
       <c r="AA63" s="14"/>
-      <c r="AB63" s="12"/>
+      <c r="AB63" s="15"/>
       <c r="AC63" s="8"/>
       <c r="AD63" s="14"/>
       <c r="AE63" s="15"/>
       <c r="AF63" s="8"/>
       <c r="AG63" s="14"/>
-      <c r="AH63" s="12"/>
+      <c r="AH63" s="15"/>
       <c r="AI63" s="8"/>
       <c r="AJ63" s="14"/>
     </row>
     <row r="64" spans="1:36">
       <c r="A64" s="20"/>
-      <c r="B64" s="31"/>
+      <c r="B64" s="20"/>
       <c r="C64" s="21"/>
       <c r="D64" s="22"/>
       <c r="E64" s="22"/>
@@ -4326,19 +4456,19 @@
       <c r="Y64" s="12"/>
       <c r="Z64" s="8"/>
       <c r="AA64" s="14"/>
-      <c r="AB64" s="12"/>
+      <c r="AB64" s="15"/>
       <c r="AC64" s="8"/>
       <c r="AD64" s="14"/>
       <c r="AE64" s="15"/>
       <c r="AF64" s="8"/>
       <c r="AG64" s="14"/>
-      <c r="AH64" s="12"/>
+      <c r="AH64" s="15"/>
       <c r="AI64" s="8"/>
       <c r="AJ64" s="14"/>
     </row>
     <row r="65" spans="1:36">
       <c r="A65" s="20"/>
-      <c r="B65" s="31"/>
+      <c r="B65" s="23"/>
       <c r="C65" s="21"/>
       <c r="D65" s="30"/>
       <c r="E65" s="30"/>
@@ -4364,57 +4494,57 @@
       <c r="Y65" s="12"/>
       <c r="Z65" s="8"/>
       <c r="AA65" s="14"/>
-      <c r="AB65" s="12"/>
+      <c r="AB65" s="15"/>
       <c r="AC65" s="8"/>
       <c r="AD65" s="14"/>
       <c r="AE65" s="15"/>
       <c r="AF65" s="8"/>
       <c r="AG65" s="14"/>
-      <c r="AH65" s="12"/>
+      <c r="AH65" s="15"/>
       <c r="AI65" s="8"/>
       <c r="AJ65" s="14"/>
     </row>
-    <row r="66" spans="1:36" s="1" customFormat="1">
-      <c r="A66" s="20"/>
-      <c r="B66" s="31"/>
-      <c r="C66" s="21"/>
+    <row r="66" spans="1:36">
+      <c r="A66" s="23"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="25"/>
       <c r="D66" s="22"/>
       <c r="E66" s="22"/>
       <c r="F66" s="65"/>
-      <c r="G66" s="12"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="15"/>
-      <c r="K66" s="8"/>
-      <c r="L66" s="14"/>
-      <c r="M66" s="12"/>
-      <c r="N66" s="8"/>
-      <c r="O66" s="14"/>
-      <c r="P66" s="15"/>
-      <c r="Q66" s="8"/>
-      <c r="R66" s="14"/>
-      <c r="S66" s="15"/>
-      <c r="T66" s="8"/>
-      <c r="U66" s="14"/>
-      <c r="V66" s="15"/>
-      <c r="W66" s="8"/>
-      <c r="X66" s="14"/>
-      <c r="Y66" s="12"/>
-      <c r="Z66" s="8"/>
-      <c r="AA66" s="14"/>
-      <c r="AB66" s="12"/>
+      <c r="G66" s="26"/>
+      <c r="H66" s="27"/>
+      <c r="I66" s="28"/>
+      <c r="J66" s="29"/>
+      <c r="K66" s="27"/>
+      <c r="L66" s="28"/>
+      <c r="M66" s="26"/>
+      <c r="N66" s="27"/>
+      <c r="O66" s="28"/>
+      <c r="P66" s="29"/>
+      <c r="Q66" s="27"/>
+      <c r="R66" s="28"/>
+      <c r="S66" s="29"/>
+      <c r="T66" s="27"/>
+      <c r="U66" s="28"/>
+      <c r="V66" s="29"/>
+      <c r="W66" s="27"/>
+      <c r="X66" s="28"/>
+      <c r="Y66" s="26"/>
+      <c r="Z66" s="27"/>
+      <c r="AA66" s="28"/>
+      <c r="AB66" s="15"/>
       <c r="AC66" s="8"/>
       <c r="AD66" s="14"/>
-      <c r="AE66" s="15"/>
-      <c r="AF66" s="8"/>
-      <c r="AG66" s="14"/>
-      <c r="AH66" s="12"/>
+      <c r="AE66" s="29"/>
+      <c r="AF66" s="27"/>
+      <c r="AG66" s="28"/>
+      <c r="AH66" s="15"/>
       <c r="AI66" s="8"/>
       <c r="AJ66" s="14"/>
     </row>
     <row r="67" spans="1:36">
       <c r="A67" s="20"/>
-      <c r="B67" s="20"/>
+      <c r="B67" s="31"/>
       <c r="C67" s="21"/>
       <c r="D67" s="30"/>
       <c r="E67" s="30"/>
@@ -4446,13 +4576,13 @@
       <c r="AE67" s="15"/>
       <c r="AF67" s="8"/>
       <c r="AG67" s="14"/>
-      <c r="AH67" s="12"/>
+      <c r="AH67" s="15"/>
       <c r="AI67" s="8"/>
       <c r="AJ67" s="14"/>
     </row>
     <row r="68" spans="1:36">
       <c r="A68" s="20"/>
-      <c r="B68" s="20"/>
+      <c r="B68" s="31"/>
       <c r="C68" s="21"/>
       <c r="D68" s="22"/>
       <c r="E68" s="22"/>
@@ -4484,49 +4614,49 @@
       <c r="AE68" s="15"/>
       <c r="AF68" s="8"/>
       <c r="AG68" s="14"/>
-      <c r="AH68" s="12"/>
+      <c r="AH68" s="15"/>
       <c r="AI68" s="8"/>
       <c r="AJ68" s="14"/>
     </row>
     <row r="69" spans="1:36">
-      <c r="A69" s="23"/>
-      <c r="B69" s="24"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="65"/>
-      <c r="G69" s="26"/>
-      <c r="H69" s="27"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="29"/>
-      <c r="K69" s="27"/>
-      <c r="L69" s="28"/>
-      <c r="M69" s="26"/>
-      <c r="N69" s="27"/>
-      <c r="O69" s="28"/>
-      <c r="P69" s="29"/>
-      <c r="Q69" s="27"/>
-      <c r="R69" s="28"/>
-      <c r="S69" s="29"/>
-      <c r="T69" s="27"/>
-      <c r="U69" s="28"/>
-      <c r="V69" s="29"/>
-      <c r="W69" s="27"/>
-      <c r="X69" s="28"/>
-      <c r="Y69" s="26"/>
-      <c r="Z69" s="27"/>
-      <c r="AA69" s="28"/>
-      <c r="AB69" s="26"/>
-      <c r="AC69" s="27"/>
-      <c r="AD69" s="28"/>
-      <c r="AE69" s="29"/>
-      <c r="AF69" s="27"/>
-      <c r="AG69" s="28"/>
-      <c r="AH69" s="26"/>
-      <c r="AI69" s="27"/>
-      <c r="AJ69" s="28"/>
-    </row>
-    <row r="70" spans="1:36" s="1" customFormat="1">
+      <c r="A69" s="20"/>
+      <c r="B69" s="31"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="64"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="8"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="12"/>
+      <c r="N69" s="8"/>
+      <c r="O69" s="14"/>
+      <c r="P69" s="15"/>
+      <c r="Q69" s="8"/>
+      <c r="R69" s="14"/>
+      <c r="S69" s="15"/>
+      <c r="T69" s="8"/>
+      <c r="U69" s="14"/>
+      <c r="V69" s="15"/>
+      <c r="W69" s="8"/>
+      <c r="X69" s="14"/>
+      <c r="Y69" s="12"/>
+      <c r="Z69" s="8"/>
+      <c r="AA69" s="14"/>
+      <c r="AB69" s="12"/>
+      <c r="AC69" s="8"/>
+      <c r="AD69" s="14"/>
+      <c r="AE69" s="15"/>
+      <c r="AF69" s="8"/>
+      <c r="AG69" s="14"/>
+      <c r="AH69" s="12"/>
+      <c r="AI69" s="8"/>
+      <c r="AJ69" s="14"/>
+    </row>
+    <row r="70" spans="1:36">
       <c r="A70" s="20"/>
       <c r="B70" s="31"/>
       <c r="C70" s="21"/>
@@ -4602,13 +4732,13 @@
       <c r="AI71" s="8"/>
       <c r="AJ71" s="14"/>
     </row>
-    <row r="72" spans="1:36">
+    <row r="72" spans="1:36" s="1" customFormat="1">
       <c r="A72" s="20"/>
-      <c r="B72" s="20"/>
+      <c r="B72" s="31"/>
       <c r="C72" s="21"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="64"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="65"/>
       <c r="G72" s="12"/>
       <c r="H72" s="8"/>
       <c r="I72" s="14"/>
@@ -4641,50 +4771,50 @@
       <c r="AJ72" s="14"/>
     </row>
     <row r="73" spans="1:36">
-      <c r="A73" s="23"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="26"/>
-      <c r="H73" s="27"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="29"/>
-      <c r="K73" s="27"/>
-      <c r="L73" s="28"/>
-      <c r="M73" s="26"/>
-      <c r="N73" s="27"/>
-      <c r="O73" s="28"/>
-      <c r="P73" s="29"/>
-      <c r="Q73" s="27"/>
-      <c r="R73" s="28"/>
-      <c r="S73" s="29"/>
-      <c r="T73" s="27"/>
-      <c r="U73" s="28"/>
-      <c r="V73" s="29"/>
-      <c r="W73" s="27"/>
-      <c r="X73" s="28"/>
-      <c r="Y73" s="26"/>
-      <c r="Z73" s="27"/>
-      <c r="AA73" s="28"/>
-      <c r="AB73" s="26"/>
-      <c r="AC73" s="27"/>
-      <c r="AD73" s="28"/>
-      <c r="AE73" s="29"/>
-      <c r="AF73" s="27"/>
-      <c r="AG73" s="28"/>
-      <c r="AH73" s="26"/>
-      <c r="AI73" s="27"/>
-      <c r="AJ73" s="28"/>
+      <c r="A73" s="20"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="30"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="8"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="12"/>
+      <c r="N73" s="8"/>
+      <c r="O73" s="14"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="8"/>
+      <c r="R73" s="14"/>
+      <c r="S73" s="15"/>
+      <c r="T73" s="8"/>
+      <c r="U73" s="14"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="8"/>
+      <c r="X73" s="14"/>
+      <c r="Y73" s="12"/>
+      <c r="Z73" s="8"/>
+      <c r="AA73" s="14"/>
+      <c r="AB73" s="12"/>
+      <c r="AC73" s="8"/>
+      <c r="AD73" s="14"/>
+      <c r="AE73" s="15"/>
+      <c r="AF73" s="8"/>
+      <c r="AG73" s="14"/>
+      <c r="AH73" s="12"/>
+      <c r="AI73" s="8"/>
+      <c r="AJ73" s="14"/>
     </row>
     <row r="74" spans="1:36">
       <c r="A74" s="20"/>
-      <c r="B74" s="31"/>
+      <c r="B74" s="20"/>
       <c r="C74" s="21"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="64"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="65"/>
       <c r="G74" s="12"/>
       <c r="H74" s="8"/>
       <c r="I74" s="14"/>
@@ -4717,44 +4847,44 @@
       <c r="AJ74" s="14"/>
     </row>
     <row r="75" spans="1:36">
-      <c r="A75" s="20"/>
-      <c r="B75" s="31"/>
-      <c r="C75" s="21"/>
+      <c r="A75" s="23"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="25"/>
       <c r="D75" s="22"/>
       <c r="E75" s="22"/>
       <c r="F75" s="65"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="14"/>
-      <c r="J75" s="15"/>
-      <c r="K75" s="8"/>
-      <c r="L75" s="14"/>
-      <c r="M75" s="12"/>
-      <c r="N75" s="8"/>
-      <c r="O75" s="14"/>
-      <c r="P75" s="15"/>
-      <c r="Q75" s="8"/>
-      <c r="R75" s="14"/>
-      <c r="S75" s="15"/>
-      <c r="T75" s="8"/>
-      <c r="U75" s="14"/>
-      <c r="V75" s="15"/>
-      <c r="W75" s="8"/>
-      <c r="X75" s="14"/>
-      <c r="Y75" s="12"/>
-      <c r="Z75" s="8"/>
-      <c r="AA75" s="14"/>
-      <c r="AB75" s="12"/>
-      <c r="AC75" s="8"/>
-      <c r="AD75" s="14"/>
-      <c r="AE75" s="15"/>
-      <c r="AF75" s="8"/>
-      <c r="AG75" s="14"/>
-      <c r="AH75" s="12"/>
-      <c r="AI75" s="8"/>
-      <c r="AJ75" s="14"/>
-    </row>
-    <row r="76" spans="1:36">
+      <c r="G75" s="26"/>
+      <c r="H75" s="27"/>
+      <c r="I75" s="28"/>
+      <c r="J75" s="29"/>
+      <c r="K75" s="27"/>
+      <c r="L75" s="28"/>
+      <c r="M75" s="26"/>
+      <c r="N75" s="27"/>
+      <c r="O75" s="28"/>
+      <c r="P75" s="29"/>
+      <c r="Q75" s="27"/>
+      <c r="R75" s="28"/>
+      <c r="S75" s="29"/>
+      <c r="T75" s="27"/>
+      <c r="U75" s="28"/>
+      <c r="V75" s="29"/>
+      <c r="W75" s="27"/>
+      <c r="X75" s="28"/>
+      <c r="Y75" s="26"/>
+      <c r="Z75" s="27"/>
+      <c r="AA75" s="28"/>
+      <c r="AB75" s="26"/>
+      <c r="AC75" s="27"/>
+      <c r="AD75" s="28"/>
+      <c r="AE75" s="29"/>
+      <c r="AF75" s="27"/>
+      <c r="AG75" s="28"/>
+      <c r="AH75" s="26"/>
+      <c r="AI75" s="27"/>
+      <c r="AJ75" s="28"/>
+    </row>
+    <row r="76" spans="1:36" s="1" customFormat="1">
       <c r="A76" s="20"/>
       <c r="B76" s="31"/>
       <c r="C76" s="21"/>
@@ -4792,7 +4922,7 @@
       <c r="AI76" s="8"/>
       <c r="AJ76" s="14"/>
     </row>
-    <row r="77" spans="1:36" s="1" customFormat="1">
+    <row r="77" spans="1:36">
       <c r="A77" s="20"/>
       <c r="B77" s="31"/>
       <c r="C77" s="21"/>
@@ -4832,11 +4962,11 @@
     </row>
     <row r="78" spans="1:36">
       <c r="A78" s="20"/>
-      <c r="B78" s="31"/>
+      <c r="B78" s="20"/>
       <c r="C78" s="21"/>
-      <c r="D78" s="22"/>
-      <c r="E78" s="22"/>
-      <c r="F78" s="65"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="30"/>
+      <c r="F78" s="64"/>
       <c r="G78" s="12"/>
       <c r="H78" s="8"/>
       <c r="I78" s="14"/>
@@ -4869,88 +4999,88 @@
       <c r="AJ78" s="14"/>
     </row>
     <row r="79" spans="1:36">
-      <c r="A79" s="20"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="30"/>
-      <c r="E79" s="30"/>
-      <c r="F79" s="64"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="8"/>
-      <c r="I79" s="14"/>
-      <c r="J79" s="15"/>
-      <c r="K79" s="8"/>
-      <c r="L79" s="14"/>
-      <c r="M79" s="12"/>
-      <c r="N79" s="8"/>
-      <c r="O79" s="14"/>
-      <c r="P79" s="15"/>
-      <c r="Q79" s="8"/>
-      <c r="R79" s="14"/>
-      <c r="S79" s="15"/>
-      <c r="T79" s="8"/>
-      <c r="U79" s="14"/>
-      <c r="V79" s="15"/>
-      <c r="W79" s="8"/>
-      <c r="X79" s="14"/>
-      <c r="Y79" s="12"/>
-      <c r="Z79" s="8"/>
-      <c r="AA79" s="14"/>
-      <c r="AB79" s="12"/>
-      <c r="AC79" s="8"/>
-      <c r="AD79" s="14"/>
-      <c r="AE79" s="15"/>
-      <c r="AF79" s="8"/>
-      <c r="AG79" s="14"/>
-      <c r="AH79" s="12"/>
-      <c r="AI79" s="8"/>
-      <c r="AJ79" s="14"/>
+      <c r="A79" s="23"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="25"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="65"/>
+      <c r="G79" s="26"/>
+      <c r="H79" s="27"/>
+      <c r="I79" s="28"/>
+      <c r="J79" s="29"/>
+      <c r="K79" s="27"/>
+      <c r="L79" s="28"/>
+      <c r="M79" s="26"/>
+      <c r="N79" s="27"/>
+      <c r="O79" s="28"/>
+      <c r="P79" s="29"/>
+      <c r="Q79" s="27"/>
+      <c r="R79" s="28"/>
+      <c r="S79" s="29"/>
+      <c r="T79" s="27"/>
+      <c r="U79" s="28"/>
+      <c r="V79" s="29"/>
+      <c r="W79" s="27"/>
+      <c r="X79" s="28"/>
+      <c r="Y79" s="26"/>
+      <c r="Z79" s="27"/>
+      <c r="AA79" s="28"/>
+      <c r="AB79" s="26"/>
+      <c r="AC79" s="27"/>
+      <c r="AD79" s="28"/>
+      <c r="AE79" s="29"/>
+      <c r="AF79" s="27"/>
+      <c r="AG79" s="28"/>
+      <c r="AH79" s="26"/>
+      <c r="AI79" s="27"/>
+      <c r="AJ79" s="28"/>
     </row>
     <row r="80" spans="1:36">
-      <c r="A80" s="23"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="65"/>
-      <c r="G80" s="26"/>
-      <c r="H80" s="27"/>
-      <c r="I80" s="28"/>
-      <c r="J80" s="29"/>
-      <c r="K80" s="27"/>
-      <c r="L80" s="28"/>
-      <c r="M80" s="26"/>
-      <c r="N80" s="27"/>
-      <c r="O80" s="28"/>
-      <c r="P80" s="29"/>
-      <c r="Q80" s="27"/>
-      <c r="R80" s="28"/>
-      <c r="S80" s="29"/>
-      <c r="T80" s="27"/>
-      <c r="U80" s="28"/>
-      <c r="V80" s="29"/>
-      <c r="W80" s="27"/>
-      <c r="X80" s="28"/>
-      <c r="Y80" s="26"/>
-      <c r="Z80" s="27"/>
-      <c r="AA80" s="28"/>
-      <c r="AB80" s="26"/>
-      <c r="AC80" s="27"/>
-      <c r="AD80" s="28"/>
-      <c r="AE80" s="29"/>
-      <c r="AF80" s="27"/>
-      <c r="AG80" s="28"/>
-      <c r="AH80" s="26"/>
-      <c r="AI80" s="27"/>
-      <c r="AJ80" s="28"/>
+      <c r="A80" s="20"/>
+      <c r="B80" s="31"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="30"/>
+      <c r="F80" s="64"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="8"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="12"/>
+      <c r="N80" s="8"/>
+      <c r="O80" s="14"/>
+      <c r="P80" s="15"/>
+      <c r="Q80" s="8"/>
+      <c r="R80" s="14"/>
+      <c r="S80" s="15"/>
+      <c r="T80" s="8"/>
+      <c r="U80" s="14"/>
+      <c r="V80" s="15"/>
+      <c r="W80" s="8"/>
+      <c r="X80" s="14"/>
+      <c r="Y80" s="12"/>
+      <c r="Z80" s="8"/>
+      <c r="AA80" s="14"/>
+      <c r="AB80" s="12"/>
+      <c r="AC80" s="8"/>
+      <c r="AD80" s="14"/>
+      <c r="AE80" s="15"/>
+      <c r="AF80" s="8"/>
+      <c r="AG80" s="14"/>
+      <c r="AH80" s="12"/>
+      <c r="AI80" s="8"/>
+      <c r="AJ80" s="14"/>
     </row>
     <row r="81" spans="1:36">
       <c r="A81" s="20"/>
       <c r="B81" s="31"/>
       <c r="C81" s="21"/>
-      <c r="D81" s="30"/>
-      <c r="E81" s="30"/>
-      <c r="F81" s="64"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="65"/>
       <c r="G81" s="12"/>
       <c r="H81" s="8"/>
       <c r="I81" s="14"/>
@@ -4982,7 +5112,7 @@
       <c r="AI81" s="8"/>
       <c r="AJ81" s="14"/>
     </row>
-    <row r="82" spans="1:36" s="1" customFormat="1">
+    <row r="82" spans="1:36">
       <c r="A82" s="20"/>
       <c r="B82" s="31"/>
       <c r="C82" s="21"/>
@@ -5020,7 +5150,7 @@
       <c r="AI82" s="8"/>
       <c r="AJ82" s="14"/>
     </row>
-    <row r="83" spans="1:36">
+    <row r="83" spans="1:36" s="1" customFormat="1">
       <c r="A83" s="20"/>
       <c r="B83" s="31"/>
       <c r="C83" s="21"/>
@@ -5060,11 +5190,11 @@
     </row>
     <row r="84" spans="1:36">
       <c r="A84" s="20"/>
-      <c r="B84" s="20"/>
+      <c r="B84" s="31"/>
       <c r="C84" s="21"/>
-      <c r="D84" s="30"/>
-      <c r="E84" s="30"/>
-      <c r="F84" s="64"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="65"/>
       <c r="G84" s="12"/>
       <c r="H84" s="8"/>
       <c r="I84" s="14"/>
@@ -5097,88 +5227,88 @@
       <c r="AJ84" s="14"/>
     </row>
     <row r="85" spans="1:36">
-      <c r="A85" s="23"/>
-      <c r="B85" s="24"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="65"/>
-      <c r="G85" s="26"/>
-      <c r="H85" s="27"/>
-      <c r="I85" s="28"/>
-      <c r="J85" s="29"/>
-      <c r="K85" s="27"/>
-      <c r="L85" s="28"/>
-      <c r="M85" s="26"/>
-      <c r="N85" s="27"/>
-      <c r="O85" s="28"/>
-      <c r="P85" s="29"/>
-      <c r="Q85" s="27"/>
-      <c r="R85" s="28"/>
-      <c r="S85" s="29"/>
-      <c r="T85" s="27"/>
-      <c r="U85" s="28"/>
-      <c r="V85" s="29"/>
-      <c r="W85" s="27"/>
-      <c r="X85" s="28"/>
-      <c r="Y85" s="26"/>
-      <c r="Z85" s="27"/>
-      <c r="AA85" s="28"/>
-      <c r="AB85" s="26"/>
-      <c r="AC85" s="27"/>
-      <c r="AD85" s="28"/>
-      <c r="AE85" s="29"/>
-      <c r="AF85" s="27"/>
-      <c r="AG85" s="28"/>
-      <c r="AH85" s="26"/>
-      <c r="AI85" s="27"/>
-      <c r="AJ85" s="28"/>
+      <c r="A85" s="20"/>
+      <c r="B85" s="20"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="30"/>
+      <c r="F85" s="64"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="15"/>
+      <c r="K85" s="8"/>
+      <c r="L85" s="14"/>
+      <c r="M85" s="12"/>
+      <c r="N85" s="8"/>
+      <c r="O85" s="14"/>
+      <c r="P85" s="15"/>
+      <c r="Q85" s="8"/>
+      <c r="R85" s="14"/>
+      <c r="S85" s="15"/>
+      <c r="T85" s="8"/>
+      <c r="U85" s="14"/>
+      <c r="V85" s="15"/>
+      <c r="W85" s="8"/>
+      <c r="X85" s="14"/>
+      <c r="Y85" s="12"/>
+      <c r="Z85" s="8"/>
+      <c r="AA85" s="14"/>
+      <c r="AB85" s="12"/>
+      <c r="AC85" s="8"/>
+      <c r="AD85" s="14"/>
+      <c r="AE85" s="15"/>
+      <c r="AF85" s="8"/>
+      <c r="AG85" s="14"/>
+      <c r="AH85" s="12"/>
+      <c r="AI85" s="8"/>
+      <c r="AJ85" s="14"/>
     </row>
     <row r="86" spans="1:36">
-      <c r="A86" s="20"/>
-      <c r="B86" s="31"/>
-      <c r="C86" s="21"/>
-      <c r="D86" s="30"/>
-      <c r="E86" s="30"/>
-      <c r="F86" s="64"/>
-      <c r="G86" s="12"/>
-      <c r="H86" s="8"/>
-      <c r="I86" s="14"/>
-      <c r="J86" s="15"/>
-      <c r="K86" s="8"/>
-      <c r="L86" s="14"/>
-      <c r="M86" s="12"/>
-      <c r="N86" s="8"/>
-      <c r="O86" s="14"/>
-      <c r="P86" s="15"/>
-      <c r="Q86" s="8"/>
-      <c r="R86" s="14"/>
-      <c r="S86" s="15"/>
-      <c r="T86" s="8"/>
-      <c r="U86" s="14"/>
-      <c r="V86" s="15"/>
-      <c r="W86" s="8"/>
-      <c r="X86" s="14"/>
-      <c r="Y86" s="12"/>
-      <c r="Z86" s="8"/>
-      <c r="AA86" s="14"/>
-      <c r="AB86" s="12"/>
-      <c r="AC86" s="8"/>
-      <c r="AD86" s="14"/>
-      <c r="AE86" s="15"/>
-      <c r="AF86" s="8"/>
-      <c r="AG86" s="14"/>
-      <c r="AH86" s="12"/>
-      <c r="AI86" s="8"/>
-      <c r="AJ86" s="14"/>
+      <c r="A86" s="23"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="25"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="65"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="27"/>
+      <c r="I86" s="28"/>
+      <c r="J86" s="29"/>
+      <c r="K86" s="27"/>
+      <c r="L86" s="28"/>
+      <c r="M86" s="26"/>
+      <c r="N86" s="27"/>
+      <c r="O86" s="28"/>
+      <c r="P86" s="29"/>
+      <c r="Q86" s="27"/>
+      <c r="R86" s="28"/>
+      <c r="S86" s="29"/>
+      <c r="T86" s="27"/>
+      <c r="U86" s="28"/>
+      <c r="V86" s="29"/>
+      <c r="W86" s="27"/>
+      <c r="X86" s="28"/>
+      <c r="Y86" s="26"/>
+      <c r="Z86" s="27"/>
+      <c r="AA86" s="28"/>
+      <c r="AB86" s="26"/>
+      <c r="AC86" s="27"/>
+      <c r="AD86" s="28"/>
+      <c r="AE86" s="29"/>
+      <c r="AF86" s="27"/>
+      <c r="AG86" s="28"/>
+      <c r="AH86" s="26"/>
+      <c r="AI86" s="27"/>
+      <c r="AJ86" s="28"/>
     </row>
     <row r="87" spans="1:36">
       <c r="A87" s="20"/>
       <c r="B87" s="31"/>
       <c r="C87" s="21"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="22"/>
-      <c r="F87" s="65"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="64"/>
       <c r="G87" s="12"/>
       <c r="H87" s="8"/>
       <c r="I87" s="14"/>
@@ -5210,13 +5340,13 @@
       <c r="AI87" s="8"/>
       <c r="AJ87" s="14"/>
     </row>
-    <row r="88" spans="1:36">
+    <row r="88" spans="1:36" s="1" customFormat="1">
       <c r="A88" s="20"/>
       <c r="B88" s="31"/>
       <c r="C88" s="21"/>
-      <c r="D88" s="30"/>
-      <c r="E88" s="30"/>
-      <c r="F88" s="64"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="22"/>
+      <c r="F88" s="65"/>
       <c r="G88" s="12"/>
       <c r="H88" s="8"/>
       <c r="I88" s="14"/>
@@ -5249,142 +5379,232 @@
       <c r="AJ88" s="14"/>
     </row>
     <row r="89" spans="1:36">
-      <c r="D89" s="18">
-        <v>1</v>
-      </c>
-      <c r="E89" s="18"/>
-      <c r="F89" s="66"/>
-      <c r="I89" s="10"/>
-      <c r="J89" s="13"/>
-      <c r="L89" s="10"/>
-      <c r="M89" s="7"/>
-      <c r="O89" s="10"/>
-      <c r="P89" s="13"/>
-      <c r="R89" s="10"/>
-      <c r="S89" s="13"/>
-      <c r="U89" s="10"/>
-      <c r="V89" s="13"/>
-      <c r="X89" s="10"/>
-      <c r="Y89" s="7"/>
-      <c r="AA89" s="10"/>
-      <c r="AB89" s="7"/>
-      <c r="AD89" s="10"/>
-      <c r="AE89" s="13"/>
+      <c r="A89" s="20"/>
+      <c r="B89" s="31"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="30"/>
+      <c r="F89" s="64"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="15"/>
+      <c r="K89" s="8"/>
+      <c r="L89" s="14"/>
+      <c r="M89" s="12"/>
+      <c r="N89" s="8"/>
+      <c r="O89" s="14"/>
+      <c r="P89" s="15"/>
+      <c r="Q89" s="8"/>
+      <c r="R89" s="14"/>
+      <c r="S89" s="15"/>
+      <c r="T89" s="8"/>
+      <c r="U89" s="14"/>
+      <c r="V89" s="15"/>
+      <c r="W89" s="8"/>
+      <c r="X89" s="14"/>
+      <c r="Y89" s="12"/>
+      <c r="Z89" s="8"/>
+      <c r="AA89" s="14"/>
+      <c r="AB89" s="12"/>
+      <c r="AC89" s="8"/>
+      <c r="AD89" s="14"/>
+      <c r="AE89" s="15"/>
+      <c r="AF89" s="8"/>
+      <c r="AG89" s="14"/>
+      <c r="AH89" s="12"/>
+      <c r="AI89" s="8"/>
+      <c r="AJ89" s="14"/>
     </row>
     <row r="90" spans="1:36">
-      <c r="D90" s="19">
-        <v>1</v>
-      </c>
-      <c r="E90" s="19"/>
-      <c r="F90" s="67"/>
-      <c r="I90" s="10"/>
-      <c r="J90" s="13"/>
-      <c r="L90" s="10"/>
-      <c r="M90" s="7"/>
-      <c r="O90" s="10"/>
-      <c r="P90" s="13"/>
-      <c r="R90" s="10"/>
-      <c r="S90" s="13"/>
-      <c r="U90" s="10"/>
-      <c r="V90" s="13"/>
-      <c r="X90" s="10"/>
-      <c r="Y90" s="7"/>
-      <c r="AA90" s="10"/>
-      <c r="AB90" s="7"/>
-      <c r="AD90" s="10"/>
-      <c r="AE90" s="13"/>
+      <c r="A90" s="20"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="21"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="30"/>
+      <c r="F90" s="64"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="8"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="15"/>
+      <c r="K90" s="8"/>
+      <c r="L90" s="14"/>
+      <c r="M90" s="12"/>
+      <c r="N90" s="8"/>
+      <c r="O90" s="14"/>
+      <c r="P90" s="15"/>
+      <c r="Q90" s="8"/>
+      <c r="R90" s="14"/>
+      <c r="S90" s="15"/>
+      <c r="T90" s="8"/>
+      <c r="U90" s="14"/>
+      <c r="V90" s="15"/>
+      <c r="W90" s="8"/>
+      <c r="X90" s="14"/>
+      <c r="Y90" s="12"/>
+      <c r="Z90" s="8"/>
+      <c r="AA90" s="14"/>
+      <c r="AB90" s="12"/>
+      <c r="AC90" s="8"/>
+      <c r="AD90" s="14"/>
+      <c r="AE90" s="15"/>
+      <c r="AF90" s="8"/>
+      <c r="AG90" s="14"/>
+      <c r="AH90" s="12"/>
+      <c r="AI90" s="8"/>
+      <c r="AJ90" s="14"/>
     </row>
     <row r="91" spans="1:36">
-      <c r="D91" s="18">
-        <v>1</v>
-      </c>
-      <c r="E91" s="18"/>
-      <c r="F91" s="66"/>
-      <c r="I91" s="10"/>
-      <c r="J91" s="13"/>
-      <c r="L91" s="10"/>
-      <c r="M91" s="7"/>
-      <c r="O91" s="10"/>
-      <c r="P91" s="13"/>
-      <c r="R91" s="10"/>
-      <c r="S91" s="13"/>
-      <c r="U91" s="10"/>
-      <c r="V91" s="13"/>
-      <c r="X91" s="10"/>
-      <c r="Y91" s="7"/>
-      <c r="AA91" s="10"/>
-      <c r="AB91" s="7"/>
-      <c r="AD91" s="10"/>
-      <c r="AE91" s="13"/>
+      <c r="A91" s="23"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="25"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="22"/>
+      <c r="F91" s="65"/>
+      <c r="G91" s="26"/>
+      <c r="H91" s="27"/>
+      <c r="I91" s="28"/>
+      <c r="J91" s="29"/>
+      <c r="K91" s="27"/>
+      <c r="L91" s="28"/>
+      <c r="M91" s="26"/>
+      <c r="N91" s="27"/>
+      <c r="O91" s="28"/>
+      <c r="P91" s="29"/>
+      <c r="Q91" s="27"/>
+      <c r="R91" s="28"/>
+      <c r="S91" s="29"/>
+      <c r="T91" s="27"/>
+      <c r="U91" s="28"/>
+      <c r="V91" s="29"/>
+      <c r="W91" s="27"/>
+      <c r="X91" s="28"/>
+      <c r="Y91" s="26"/>
+      <c r="Z91" s="27"/>
+      <c r="AA91" s="28"/>
+      <c r="AB91" s="26"/>
+      <c r="AC91" s="27"/>
+      <c r="AD91" s="28"/>
+      <c r="AE91" s="29"/>
+      <c r="AF91" s="27"/>
+      <c r="AG91" s="28"/>
+      <c r="AH91" s="26"/>
+      <c r="AI91" s="27"/>
+      <c r="AJ91" s="28"/>
     </row>
     <row r="92" spans="1:36">
-      <c r="D92" s="19">
-        <v>1</v>
-      </c>
-      <c r="E92" s="19"/>
-      <c r="F92" s="67"/>
-      <c r="I92" s="10"/>
-      <c r="J92" s="13"/>
-      <c r="L92" s="10"/>
-      <c r="M92" s="7"/>
-      <c r="O92" s="10"/>
-      <c r="P92" s="13"/>
-      <c r="R92" s="10"/>
-      <c r="S92" s="13"/>
-      <c r="U92" s="10"/>
-      <c r="V92" s="13"/>
-      <c r="X92" s="10"/>
-      <c r="Y92" s="7"/>
-      <c r="AA92" s="10"/>
-      <c r="AB92" s="7"/>
-      <c r="AD92" s="10"/>
-      <c r="AE92" s="13"/>
+      <c r="A92" s="20"/>
+      <c r="B92" s="31"/>
+      <c r="C92" s="21"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="30"/>
+      <c r="F92" s="64"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="8"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="8"/>
+      <c r="L92" s="14"/>
+      <c r="M92" s="12"/>
+      <c r="N92" s="8"/>
+      <c r="O92" s="14"/>
+      <c r="P92" s="15"/>
+      <c r="Q92" s="8"/>
+      <c r="R92" s="14"/>
+      <c r="S92" s="15"/>
+      <c r="T92" s="8"/>
+      <c r="U92" s="14"/>
+      <c r="V92" s="15"/>
+      <c r="W92" s="8"/>
+      <c r="X92" s="14"/>
+      <c r="Y92" s="12"/>
+      <c r="Z92" s="8"/>
+      <c r="AA92" s="14"/>
+      <c r="AB92" s="12"/>
+      <c r="AC92" s="8"/>
+      <c r="AD92" s="14"/>
+      <c r="AE92" s="15"/>
+      <c r="AF92" s="8"/>
+      <c r="AG92" s="14"/>
+      <c r="AH92" s="12"/>
+      <c r="AI92" s="8"/>
+      <c r="AJ92" s="14"/>
     </row>
     <row r="93" spans="1:36">
-      <c r="D93" s="18">
-        <v>1</v>
-      </c>
-      <c r="E93" s="18"/>
-      <c r="F93" s="66"/>
-      <c r="I93" s="10"/>
-      <c r="J93" s="13"/>
-      <c r="L93" s="10"/>
-      <c r="M93" s="7"/>
-      <c r="O93" s="10"/>
-      <c r="P93" s="13"/>
-      <c r="R93" s="10"/>
-      <c r="S93" s="13"/>
-      <c r="U93" s="10"/>
-      <c r="V93" s="13"/>
-      <c r="X93" s="10"/>
-      <c r="Y93" s="7"/>
-      <c r="AA93" s="10"/>
-      <c r="AB93" s="7"/>
-      <c r="AD93" s="10"/>
-      <c r="AE93" s="13"/>
+      <c r="A93" s="20"/>
+      <c r="B93" s="31"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="22"/>
+      <c r="F93" s="65"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="8"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="8"/>
+      <c r="L93" s="14"/>
+      <c r="M93" s="12"/>
+      <c r="N93" s="8"/>
+      <c r="O93" s="14"/>
+      <c r="P93" s="15"/>
+      <c r="Q93" s="8"/>
+      <c r="R93" s="14"/>
+      <c r="S93" s="15"/>
+      <c r="T93" s="8"/>
+      <c r="U93" s="14"/>
+      <c r="V93" s="15"/>
+      <c r="W93" s="8"/>
+      <c r="X93" s="14"/>
+      <c r="Y93" s="12"/>
+      <c r="Z93" s="8"/>
+      <c r="AA93" s="14"/>
+      <c r="AB93" s="12"/>
+      <c r="AC93" s="8"/>
+      <c r="AD93" s="14"/>
+      <c r="AE93" s="15"/>
+      <c r="AF93" s="8"/>
+      <c r="AG93" s="14"/>
+      <c r="AH93" s="12"/>
+      <c r="AI93" s="8"/>
+      <c r="AJ93" s="14"/>
     </row>
     <row r="94" spans="1:36">
-      <c r="D94" s="19">
-        <v>1</v>
-      </c>
-      <c r="E94" s="19"/>
-      <c r="F94" s="67"/>
-      <c r="I94" s="10"/>
-      <c r="J94" s="13"/>
-      <c r="L94" s="10"/>
-      <c r="M94" s="7"/>
-      <c r="O94" s="10"/>
-      <c r="P94" s="13"/>
-      <c r="R94" s="10"/>
-      <c r="S94" s="13"/>
-      <c r="U94" s="10"/>
-      <c r="V94" s="13"/>
-      <c r="X94" s="10"/>
-      <c r="Y94" s="7"/>
-      <c r="AA94" s="10"/>
-      <c r="AB94" s="7"/>
-      <c r="AD94" s="10"/>
-      <c r="AE94" s="13"/>
+      <c r="A94" s="20"/>
+      <c r="B94" s="31"/>
+      <c r="C94" s="21"/>
+      <c r="D94" s="30"/>
+      <c r="E94" s="30"/>
+      <c r="F94" s="64"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="8"/>
+      <c r="I94" s="14"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="8"/>
+      <c r="L94" s="14"/>
+      <c r="M94" s="12"/>
+      <c r="N94" s="8"/>
+      <c r="O94" s="14"/>
+      <c r="P94" s="15"/>
+      <c r="Q94" s="8"/>
+      <c r="R94" s="14"/>
+      <c r="S94" s="15"/>
+      <c r="T94" s="8"/>
+      <c r="U94" s="14"/>
+      <c r="V94" s="15"/>
+      <c r="W94" s="8"/>
+      <c r="X94" s="14"/>
+      <c r="Y94" s="12"/>
+      <c r="Z94" s="8"/>
+      <c r="AA94" s="14"/>
+      <c r="AB94" s="12"/>
+      <c r="AC94" s="8"/>
+      <c r="AD94" s="14"/>
+      <c r="AE94" s="15"/>
+      <c r="AF94" s="8"/>
+      <c r="AG94" s="14"/>
+      <c r="AH94" s="12"/>
+      <c r="AI94" s="8"/>
+      <c r="AJ94" s="14"/>
     </row>
     <row r="95" spans="1:36">
       <c r="D95" s="18">
@@ -5637,7 +5857,7 @@
       <c r="AA105" s="10"/>
       <c r="AB105" s="7"/>
       <c r="AD105" s="10"/>
-      <c r="AE105" s="7"/>
+      <c r="AE105" s="13"/>
     </row>
     <row r="106" spans="4:31">
       <c r="D106" s="19">
@@ -5660,7 +5880,7 @@
       <c r="AA106" s="10"/>
       <c r="AB106" s="7"/>
       <c r="AD106" s="10"/>
-      <c r="AE106" s="7"/>
+      <c r="AE106" s="13"/>
     </row>
     <row r="107" spans="4:31">
       <c r="D107" s="18">
@@ -5683,7 +5903,7 @@
       <c r="AA107" s="10"/>
       <c r="AB107" s="7"/>
       <c r="AD107" s="10"/>
-      <c r="AE107" s="7"/>
+      <c r="AE107" s="13"/>
     </row>
     <row r="108" spans="4:31">
       <c r="D108" s="19">
@@ -5706,7 +5926,7 @@
       <c r="AA108" s="10"/>
       <c r="AB108" s="7"/>
       <c r="AD108" s="10"/>
-      <c r="AE108" s="7"/>
+      <c r="AE108" s="13"/>
     </row>
     <row r="109" spans="4:31">
       <c r="D109" s="18">
@@ -5729,7 +5949,7 @@
       <c r="AA109" s="10"/>
       <c r="AB109" s="7"/>
       <c r="AD109" s="10"/>
-      <c r="AE109" s="7"/>
+      <c r="AE109" s="13"/>
     </row>
     <row r="110" spans="4:31">
       <c r="D110" s="19">
@@ -5752,7 +5972,7 @@
       <c r="AA110" s="10"/>
       <c r="AB110" s="7"/>
       <c r="AD110" s="10"/>
-      <c r="AE110" s="7"/>
+      <c r="AE110" s="13"/>
     </row>
     <row r="111" spans="4:31">
       <c r="D111" s="18">
@@ -5999,7 +6219,9 @@
       <c r="R121" s="10"/>
       <c r="S121" s="13"/>
       <c r="U121" s="10"/>
-      <c r="V121" s="7"/>
+      <c r="V121" s="13"/>
+      <c r="X121" s="10"/>
+      <c r="Y121" s="7"/>
       <c r="AA121" s="10"/>
       <c r="AB121" s="7"/>
       <c r="AD121" s="10"/>
@@ -6020,7 +6242,9 @@
       <c r="R122" s="10"/>
       <c r="S122" s="13"/>
       <c r="U122" s="10"/>
-      <c r="V122" s="7"/>
+      <c r="V122" s="13"/>
+      <c r="X122" s="10"/>
+      <c r="Y122" s="7"/>
       <c r="AA122" s="10"/>
       <c r="AB122" s="7"/>
       <c r="AD122" s="10"/>
@@ -6041,7 +6265,9 @@
       <c r="R123" s="10"/>
       <c r="S123" s="13"/>
       <c r="U123" s="10"/>
-      <c r="V123" s="7"/>
+      <c r="V123" s="13"/>
+      <c r="X123" s="10"/>
+      <c r="Y123" s="7"/>
       <c r="AA123" s="10"/>
       <c r="AB123" s="7"/>
       <c r="AD123" s="10"/>
@@ -6062,7 +6288,9 @@
       <c r="R124" s="10"/>
       <c r="S124" s="13"/>
       <c r="U124" s="10"/>
-      <c r="V124" s="7"/>
+      <c r="V124" s="13"/>
+      <c r="X124" s="10"/>
+      <c r="Y124" s="7"/>
       <c r="AA124" s="10"/>
       <c r="AB124" s="7"/>
       <c r="AD124" s="10"/>
@@ -6083,7 +6311,9 @@
       <c r="R125" s="10"/>
       <c r="S125" s="13"/>
       <c r="U125" s="10"/>
-      <c r="V125" s="7"/>
+      <c r="V125" s="13"/>
+      <c r="X125" s="10"/>
+      <c r="Y125" s="7"/>
       <c r="AA125" s="10"/>
       <c r="AB125" s="7"/>
       <c r="AD125" s="10"/>
@@ -6104,7 +6334,9 @@
       <c r="R126" s="10"/>
       <c r="S126" s="13"/>
       <c r="U126" s="10"/>
-      <c r="V126" s="7"/>
+      <c r="V126" s="13"/>
+      <c r="X126" s="10"/>
+      <c r="Y126" s="7"/>
       <c r="AA126" s="10"/>
       <c r="AB126" s="7"/>
       <c r="AD126" s="10"/>
@@ -6369,7 +6601,9 @@
       <c r="E139" s="18"/>
       <c r="F139" s="66"/>
       <c r="I139" s="10"/>
-      <c r="J139" s="7"/>
+      <c r="J139" s="13"/>
+      <c r="L139" s="10"/>
+      <c r="M139" s="7"/>
       <c r="O139" s="10"/>
       <c r="P139" s="13"/>
       <c r="R139" s="10"/>
@@ -6388,7 +6622,9 @@
       <c r="E140" s="19"/>
       <c r="F140" s="67"/>
       <c r="I140" s="10"/>
-      <c r="J140" s="7"/>
+      <c r="J140" s="13"/>
+      <c r="L140" s="10"/>
+      <c r="M140" s="7"/>
       <c r="O140" s="10"/>
       <c r="P140" s="13"/>
       <c r="R140" s="10"/>
@@ -6407,11 +6643,15 @@
       <c r="E141" s="18"/>
       <c r="F141" s="66"/>
       <c r="I141" s="10"/>
-      <c r="J141" s="7"/>
+      <c r="J141" s="13"/>
+      <c r="L141" s="10"/>
+      <c r="M141" s="7"/>
       <c r="O141" s="10"/>
       <c r="P141" s="13"/>
       <c r="R141" s="10"/>
-      <c r="S141" s="7"/>
+      <c r="S141" s="13"/>
+      <c r="U141" s="10"/>
+      <c r="V141" s="7"/>
       <c r="AA141" s="10"/>
       <c r="AB141" s="7"/>
       <c r="AD141" s="10"/>
@@ -6424,11 +6664,15 @@
       <c r="E142" s="19"/>
       <c r="F142" s="67"/>
       <c r="I142" s="10"/>
-      <c r="J142" s="7"/>
+      <c r="J142" s="13"/>
+      <c r="L142" s="10"/>
+      <c r="M142" s="7"/>
       <c r="O142" s="10"/>
       <c r="P142" s="13"/>
       <c r="R142" s="10"/>
-      <c r="S142" s="7"/>
+      <c r="S142" s="13"/>
+      <c r="U142" s="10"/>
+      <c r="V142" s="7"/>
       <c r="AA142" s="10"/>
       <c r="AB142" s="7"/>
       <c r="AD142" s="10"/>
@@ -6441,11 +6685,15 @@
       <c r="E143" s="18"/>
       <c r="F143" s="66"/>
       <c r="I143" s="10"/>
-      <c r="J143" s="7"/>
+      <c r="J143" s="13"/>
+      <c r="L143" s="10"/>
+      <c r="M143" s="7"/>
       <c r="O143" s="10"/>
       <c r="P143" s="13"/>
       <c r="R143" s="10"/>
-      <c r="S143" s="7"/>
+      <c r="S143" s="13"/>
+      <c r="U143" s="10"/>
+      <c r="V143" s="7"/>
       <c r="AA143" s="10"/>
       <c r="AB143" s="7"/>
       <c r="AD143" s="10"/>
@@ -6458,11 +6706,15 @@
       <c r="E144" s="19"/>
       <c r="F144" s="67"/>
       <c r="I144" s="10"/>
-      <c r="J144" s="7"/>
+      <c r="J144" s="13"/>
+      <c r="L144" s="10"/>
+      <c r="M144" s="7"/>
       <c r="O144" s="10"/>
       <c r="P144" s="13"/>
       <c r="R144" s="10"/>
-      <c r="S144" s="7"/>
+      <c r="S144" s="13"/>
+      <c r="U144" s="10"/>
+      <c r="V144" s="7"/>
       <c r="AA144" s="10"/>
       <c r="AB144" s="7"/>
       <c r="AD144" s="10"/>
@@ -6479,7 +6731,9 @@
       <c r="O145" s="10"/>
       <c r="P145" s="13"/>
       <c r="R145" s="10"/>
-      <c r="S145" s="7"/>
+      <c r="S145" s="13"/>
+      <c r="U145" s="10"/>
+      <c r="V145" s="7"/>
       <c r="AA145" s="10"/>
       <c r="AB145" s="7"/>
       <c r="AD145" s="10"/>
@@ -6496,7 +6750,9 @@
       <c r="O146" s="10"/>
       <c r="P146" s="13"/>
       <c r="R146" s="10"/>
-      <c r="S146" s="7"/>
+      <c r="S146" s="13"/>
+      <c r="U146" s="10"/>
+      <c r="V146" s="7"/>
       <c r="AA146" s="10"/>
       <c r="AB146" s="7"/>
       <c r="AD146" s="10"/>
@@ -7392,6 +7648,8 @@
       </c>
       <c r="E199" s="18"/>
       <c r="F199" s="66"/>
+      <c r="I199" s="10"/>
+      <c r="J199" s="7"/>
       <c r="O199" s="10"/>
       <c r="P199" s="13"/>
       <c r="R199" s="10"/>
@@ -7407,6 +7665,8 @@
       </c>
       <c r="E200" s="19"/>
       <c r="F200" s="67"/>
+      <c r="I200" s="10"/>
+      <c r="J200" s="7"/>
       <c r="O200" s="10"/>
       <c r="P200" s="13"/>
       <c r="R200" s="10"/>
@@ -7422,6 +7682,8 @@
       </c>
       <c r="E201" s="18"/>
       <c r="F201" s="66"/>
+      <c r="I201" s="10"/>
+      <c r="J201" s="7"/>
       <c r="O201" s="10"/>
       <c r="P201" s="13"/>
       <c r="R201" s="10"/>
@@ -7437,6 +7699,8 @@
       </c>
       <c r="E202" s="19"/>
       <c r="F202" s="67"/>
+      <c r="I202" s="10"/>
+      <c r="J202" s="7"/>
       <c r="O202" s="10"/>
       <c r="P202" s="13"/>
       <c r="R202" s="10"/>
@@ -7452,8 +7716,12 @@
       </c>
       <c r="E203" s="18"/>
       <c r="F203" s="66"/>
+      <c r="I203" s="10"/>
+      <c r="J203" s="7"/>
       <c r="O203" s="10"/>
-      <c r="P203" s="7"/>
+      <c r="P203" s="13"/>
+      <c r="R203" s="10"/>
+      <c r="S203" s="7"/>
       <c r="AA203" s="10"/>
       <c r="AB203" s="7"/>
       <c r="AD203" s="10"/>
@@ -7465,8 +7733,12 @@
       </c>
       <c r="E204" s="19"/>
       <c r="F204" s="67"/>
+      <c r="I204" s="10"/>
+      <c r="J204" s="7"/>
       <c r="O204" s="10"/>
-      <c r="P204" s="7"/>
+      <c r="P204" s="13"/>
+      <c r="R204" s="10"/>
+      <c r="S204" s="7"/>
       <c r="AA204" s="10"/>
       <c r="AB204" s="7"/>
       <c r="AD204" s="10"/>
@@ -7479,7 +7751,9 @@
       <c r="E205" s="18"/>
       <c r="F205" s="66"/>
       <c r="O205" s="10"/>
-      <c r="P205" s="7"/>
+      <c r="P205" s="13"/>
+      <c r="R205" s="10"/>
+      <c r="S205" s="7"/>
       <c r="AA205" s="10"/>
       <c r="AB205" s="7"/>
       <c r="AD205" s="10"/>
@@ -7492,7 +7766,9 @@
       <c r="E206" s="19"/>
       <c r="F206" s="67"/>
       <c r="O206" s="10"/>
-      <c r="P206" s="7"/>
+      <c r="P206" s="13"/>
+      <c r="R206" s="10"/>
+      <c r="S206" s="7"/>
       <c r="AA206" s="10"/>
       <c r="AB206" s="7"/>
       <c r="AD206" s="10"/>
@@ -7505,7 +7781,9 @@
       <c r="E207" s="18"/>
       <c r="F207" s="66"/>
       <c r="O207" s="10"/>
-      <c r="P207" s="7"/>
+      <c r="P207" s="13"/>
+      <c r="R207" s="10"/>
+      <c r="S207" s="7"/>
       <c r="AA207" s="10"/>
       <c r="AB207" s="7"/>
       <c r="AD207" s="10"/>
@@ -7518,7 +7796,9 @@
       <c r="E208" s="19"/>
       <c r="F208" s="67"/>
       <c r="O208" s="10"/>
-      <c r="P208" s="7"/>
+      <c r="P208" s="13"/>
+      <c r="R208" s="10"/>
+      <c r="S208" s="7"/>
       <c r="AA208" s="10"/>
       <c r="AB208" s="7"/>
       <c r="AD208" s="10"/>
@@ -8167,6 +8447,8 @@
       </c>
       <c r="E258" s="19"/>
       <c r="F258" s="67"/>
+      <c r="O258" s="10"/>
+      <c r="P258" s="7"/>
       <c r="AA258" s="10"/>
       <c r="AB258" s="7"/>
       <c r="AD258" s="10"/>
@@ -8178,6 +8460,10 @@
       </c>
       <c r="E259" s="18"/>
       <c r="F259" s="66"/>
+      <c r="O259" s="10"/>
+      <c r="P259" s="7"/>
+      <c r="AA259" s="10"/>
+      <c r="AB259" s="7"/>
       <c r="AD259" s="10"/>
       <c r="AE259" s="7"/>
     </row>
@@ -8187,6 +8473,10 @@
       </c>
       <c r="E260" s="19"/>
       <c r="F260" s="67"/>
+      <c r="O260" s="10"/>
+      <c r="P260" s="7"/>
+      <c r="AA260" s="10"/>
+      <c r="AB260" s="7"/>
       <c r="AD260" s="10"/>
       <c r="AE260" s="7"/>
     </row>
@@ -8196,6 +8486,10 @@
       </c>
       <c r="E261" s="18"/>
       <c r="F261" s="66"/>
+      <c r="O261" s="10"/>
+      <c r="P261" s="7"/>
+      <c r="AA261" s="10"/>
+      <c r="AB261" s="7"/>
       <c r="AD261" s="10"/>
       <c r="AE261" s="7"/>
     </row>
@@ -8205,6 +8499,10 @@
       </c>
       <c r="E262" s="19"/>
       <c r="F262" s="67"/>
+      <c r="O262" s="10"/>
+      <c r="P262" s="7"/>
+      <c r="AA262" s="10"/>
+      <c r="AB262" s="7"/>
       <c r="AD262" s="10"/>
       <c r="AE262" s="7"/>
     </row>
@@ -8214,6 +8512,10 @@
       </c>
       <c r="E263" s="18"/>
       <c r="F263" s="66"/>
+      <c r="O263" s="10"/>
+      <c r="P263" s="7"/>
+      <c r="AA263" s="10"/>
+      <c r="AB263" s="7"/>
       <c r="AD263" s="10"/>
       <c r="AE263" s="7"/>
     </row>
@@ -8223,6 +8525,8 @@
       </c>
       <c r="E264" s="19"/>
       <c r="F264" s="67"/>
+      <c r="AA264" s="10"/>
+      <c r="AB264" s="7"/>
       <c r="AD264" s="10"/>
       <c r="AE264" s="7"/>
     </row>
@@ -8367,6 +8671,8 @@
       </c>
       <c r="E280" s="19"/>
       <c r="F280" s="67"/>
+      <c r="AD280" s="10"/>
+      <c r="AE280" s="7"/>
     </row>
     <row r="281" spans="4:31">
       <c r="D281" s="18">
@@ -8374,6 +8680,8 @@
       </c>
       <c r="E281" s="18"/>
       <c r="F281" s="66"/>
+      <c r="AD281" s="10"/>
+      <c r="AE281" s="7"/>
     </row>
     <row r="282" spans="4:31">
       <c r="D282" s="19">
@@ -8381,6 +8689,8 @@
       </c>
       <c r="E282" s="19"/>
       <c r="F282" s="67"/>
+      <c r="AD282" s="10"/>
+      <c r="AE282" s="7"/>
     </row>
     <row r="283" spans="4:31">
       <c r="D283" s="18">
@@ -8388,6 +8698,8 @@
       </c>
       <c r="E283" s="18"/>
       <c r="F283" s="66"/>
+      <c r="AD283" s="10"/>
+      <c r="AE283" s="7"/>
     </row>
     <row r="284" spans="4:31">
       <c r="D284" s="19">
@@ -8395,6 +8707,8 @@
       </c>
       <c r="E284" s="19"/>
       <c r="F284" s="67"/>
+      <c r="AD284" s="10"/>
+      <c r="AE284" s="7"/>
     </row>
     <row r="285" spans="4:31">
       <c r="D285" s="18">
@@ -8402,6 +8716,8 @@
       </c>
       <c r="E285" s="18"/>
       <c r="F285" s="66"/>
+      <c r="AD285" s="10"/>
+      <c r="AE285" s="7"/>
     </row>
     <row r="286" spans="4:31">
       <c r="D286" s="19">
@@ -8675,6 +8991,48 @@
       </c>
       <c r="E324" s="19"/>
       <c r="F324" s="67"/>
+    </row>
+    <row r="325" spans="4:6">
+      <c r="D325" s="18">
+        <v>1</v>
+      </c>
+      <c r="E325" s="18"/>
+      <c r="F325" s="66"/>
+    </row>
+    <row r="326" spans="4:6">
+      <c r="D326" s="19">
+        <v>1</v>
+      </c>
+      <c r="E326" s="19"/>
+      <c r="F326" s="67"/>
+    </row>
+    <row r="327" spans="4:6">
+      <c r="D327" s="18">
+        <v>1</v>
+      </c>
+      <c r="E327" s="18"/>
+      <c r="F327" s="66"/>
+    </row>
+    <row r="328" spans="4:6">
+      <c r="D328" s="19">
+        <v>1</v>
+      </c>
+      <c r="E328" s="19"/>
+      <c r="F328" s="67"/>
+    </row>
+    <row r="329" spans="4:6">
+      <c r="D329" s="18">
+        <v>1</v>
+      </c>
+      <c r="E329" s="18"/>
+      <c r="F329" s="66"/>
+    </row>
+    <row r="330" spans="4:6">
+      <c r="D330" s="19">
+        <v>1</v>
+      </c>
+      <c r="E330" s="19"/>
+      <c r="F330" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -8698,17 +9056,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="61.1640625" customWidth="1"/>
+    <col min="1" max="1" width="61.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="32">
+    <row r="1" spans="1:1" ht="31.5">
       <c r="A1" s="51" t="s">
         <v>124</v>
       </c>
@@ -8719,16 +9077,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:C21"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:3">

</xml_diff>